<commit_message>
Updates on code list metadata to align it for next release
Partial changes applied to the code lists. A few changes are still pending and will be committed the sooner.
</commit_message>
<xml_diff>
--- a/__ESPDTeam__/ESPD-CodeLists.xlsx
+++ b/__ESPDTeam__/ESPD-CodeLists.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25726"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hricolor\Documents\GitHub\ESPD-EDM-OP-TED\__ESPDTeam__\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hricolor\Documents\GitHub\ESPD-EDM-3.1.0\__ESPDTeam__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A9B677E-13DD-4D5F-9F9F-0B2B3531E3A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DCA4BC1-6E47-497A-97B4-5C59DB1BFA3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27990" yWindow="15" windowWidth="28110" windowHeight="16440" tabRatio="884" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1035" yWindow="-16320" windowWidth="28110" windowHeight="16440" tabRatio="884" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AccessRight" sheetId="199" r:id="rId1"/>
@@ -308,7 +308,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="343">
   <si>
     <t>ListID</t>
   </si>
@@ -1189,9 +1189,6 @@
     <t>financial-ratio-type</t>
   </si>
   <si>
-    <t>20210317-0</t>
-  </si>
-  <si>
     <t>20210616-0</t>
   </si>
   <si>
@@ -1201,24 +1198,12 @@
     <t>http://publications.europa.eu/resource/distribution/criterion/20210616-0/xml/gc/Criterion.gc</t>
   </si>
   <si>
-    <t>http://publications.europa.eu/resource/dataset/economic-operator-size/20210317-0</t>
-  </si>
-  <si>
-    <t>http://publications.europa.eu/resource/distribution/economic-operator-size/20210317-0/xml/gc/EconomicOperatorSize.gc</t>
-  </si>
-  <si>
     <t>https://github.com/ESPD/ESPD-EDM/tree/v3.0.1</t>
   </si>
   <si>
     <t>20211208-0</t>
   </si>
   <si>
-    <t>http://publications.europa.eu/resource/dataset/access-right/20211208-0</t>
-  </si>
-  <si>
-    <t>http://publications.europa.eu/resource/distribution/access-right/20211208-0/xml/gc/AccessRight.gc</t>
-  </si>
-  <si>
     <t>https://github.com/ESPD/ESPD-EDM/tree/v3.0.1/codelists/gc/BooleanGUIControlType.gc</t>
   </si>
   <si>
@@ -1328,6 +1313,30 @@
   </si>
   <si>
     <t>EMPL</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 20220316-0</t>
+  </si>
+  <si>
+    <t>http://publications.europa.eu/resource/dataset/access-right/20220316-0</t>
+  </si>
+  <si>
+    <t>https://op.europa.eu/en/web/eu-vocabularies/dataset/-/resource?uri=http://publications.europa.eu/resource/dataset/access-right</t>
+  </si>
+  <si>
+    <t>20220316-0</t>
+  </si>
+  <si>
+    <t>http://publications.europa.eu/resource/dataset/economic-operator-size/20220316-0</t>
+  </si>
+  <si>
+    <t>http://publications.europa.eu/resource/distribution/economic-operator-size/20220316-0/xml/gc/EconomicOperatorSize.gc</t>
+  </si>
+  <si>
+    <t>http://publications.europa.eu/resource/authority/occupation</t>
+  </si>
+  <si>
+    <t>3.1.0</t>
   </si>
 </sst>
 </file>
@@ -7079,7 +7088,7 @@
   <dimension ref="A1:AB17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -7116,7 +7125,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>300</v>
+        <v>335</v>
       </c>
       <c r="C4" s="5"/>
     </row>
@@ -7134,7 +7143,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>301</v>
+        <v>336</v>
       </c>
       <c r="C6" s="14"/>
       <c r="F6" s="21"/>
@@ -7144,7 +7153,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>302</v>
+        <v>337</v>
       </c>
       <c r="C7" s="14"/>
     </row>
@@ -7254,42 +7263,42 @@
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="D11" t="s">
         <v>216</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="B12" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="D12" t="s">
         <v>216</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="L12" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.25">
@@ -7369,7 +7378,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="13" x14ac:dyDescent="0.3">
@@ -7385,7 +7394,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="13" x14ac:dyDescent="0.3">
@@ -7393,7 +7402,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="13" x14ac:dyDescent="0.3">
@@ -7430,7 +7439,7 @@
   <dimension ref="A1:AB38"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -7459,7 +7468,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>279</v>
+        <v>342</v>
       </c>
     </row>
     <row r="4" spans="1:28" ht="13" x14ac:dyDescent="0.3">
@@ -7475,7 +7484,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="6" spans="1:28" ht="13" x14ac:dyDescent="0.3">
@@ -7483,7 +7492,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
     </row>
     <row r="7" spans="1:28" ht="13" x14ac:dyDescent="0.3">
@@ -8495,7 +8504,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="C4" s="5"/>
     </row>
@@ -8513,7 +8522,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="C6" s="14"/>
     </row>
@@ -8522,7 +8531,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="C7" s="14"/>
     </row>
@@ -8560,8 +8569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:AB9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -8593,8 +8602,8 @@
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>268</v>
+      <c r="B3" s="14" t="s">
+        <v>341</v>
       </c>
       <c r="C3" s="5"/>
     </row>
@@ -8603,7 +8612,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="C4" s="5"/>
     </row>
@@ -8612,7 +8621,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="C5" s="14"/>
     </row>
@@ -8621,7 +8630,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="C6" s="14"/>
     </row>
@@ -8630,7 +8639,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="C7" s="14"/>
     </row>
@@ -8639,7 +8648,7 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
@@ -8673,7 +8682,7 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
     </row>
   </sheetData>
@@ -8681,9 +8690,10 @@
     <hyperlink ref="B5" r:id="rId1" xr:uid="{00000000-0004-0000-0C00-000000000000}"/>
     <hyperlink ref="B6" r:id="rId2" xr:uid="{00000000-0004-0000-0C00-000001000000}"/>
     <hyperlink ref="B7" r:id="rId3" xr:uid="{00000000-0004-0000-0C00-000002000000}"/>
+    <hyperlink ref="B3" r:id="rId4" xr:uid="{D910A4CE-5D30-4573-94E6-AC5A9DB508D1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -8693,7 +8703,7 @@
   <dimension ref="A1:AB16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -8747,7 +8757,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -8757,7 +8767,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -9013,13 +9023,13 @@
     </row>
     <row r="16" spans="1:28" ht="16" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="D16" s="16" t="s">
         <v>216</v>
@@ -9032,7 +9042,7 @@
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
       <c r="L16" s="6" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="M16" s="6"/>
       <c r="N16" s="6"/>
@@ -9116,7 +9126,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C5" s="14"/>
     </row>
@@ -9125,7 +9135,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="C6" s="14"/>
     </row>
@@ -9407,7 +9417,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C5" s="17"/>
       <c r="D5" s="17"/>
@@ -9417,7 +9427,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>
@@ -9633,10 +9643,10 @@
         <v>12</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>216</v>
@@ -9649,7 +9659,7 @@
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
       <c r="L11" s="8" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="M11" s="8"/>
       <c r="N11" s="8"/>
@@ -10565,8 +10575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AB13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -10598,7 +10608,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>279</v>
+        <v>342</v>
       </c>
       <c r="C3" s="5"/>
     </row>
@@ -10616,7 +10626,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C5" s="14"/>
     </row>
@@ -10625,7 +10635,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="C6" s="14"/>
     </row>
@@ -11015,7 +11025,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="C4" s="5"/>
     </row>
@@ -11033,7 +11043,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="C6" s="1"/>
     </row>
@@ -11042,7 +11052,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="C7" s="1"/>
     </row>
@@ -11082,7 +11092,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -11126,7 +11136,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -11146,7 +11156,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="21"/>
@@ -11156,7 +11166,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -11200,7 +11210,7 @@
   <dimension ref="A1:AB18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -11235,7 +11245,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>279</v>
+        <v>342</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -11255,7 +11265,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -11265,7 +11275,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -11769,7 +11779,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -11812,7 +11822,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -11832,7 +11842,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -11842,7 +11852,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -11921,7 +11931,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -11931,7 +11941,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -11941,7 +11951,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -11951,7 +11961,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -11961,7 +11971,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -12000,7 +12010,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -12045,7 +12055,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>293</v>
+        <v>338</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -12065,7 +12075,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>297</v>
+        <v>339</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -12075,7 +12085,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>298</v>
+        <v>340</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -12118,7 +12128,7 @@
   <dimension ref="A1:AB12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -12151,7 +12161,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>279</v>
+        <v>342</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -12171,7 +12181,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -12181,7 +12191,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -12495,6 +12505,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100087E4EC354ADFB40AC5D4FC129E379BA" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="29f822455ff5391d2c7c2dfd7717ecba">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="541a8a8b-b856-4d35-a5c7-7f2c0ec3d499" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="35e6952e7efa586d011e824f69a654f2" ns2:_="">
     <xsd:import namespace="541a8a8b-b856-4d35-a5c7-7f2c0ec3d499"/>
@@ -12666,12 +12682,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{742639C9-D5E0-4CBF-8139-6F41798C6819}">
   <ds:schemaRefs>
@@ -12681,6 +12691,22 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E61FB905-6753-4D6B-9555-45A818BB6BAA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="541a8a8b-b856-4d35-a5c7-7f2c0ec3d499"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5774DC4B-7AB9-4854-9E79-56DDD4D64737}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12696,20 +12722,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E61FB905-6753-4D6B-9555-45A818BB6BAA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="541a8a8b-b856-4d35-a5c7-7f2c0ec3d499"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
CL update - alignment with validation artefacts
</commit_message>
<xml_diff>
--- a/__ESPDTeam__/ESPD-CodeLists.xlsx
+++ b/__ESPDTeam__/ESPD-CodeLists.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hricolor\Documents\GitHub\ESPD-EDM-3.1.0\__ESPDTeam__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DCA4BC1-6E47-497A-97B4-5C59DB1BFA3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8E76DE-301C-46D2-A2EE-AFDFB4E95C98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1035" yWindow="-16320" windowWidth="28110" windowHeight="16440" tabRatio="884" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="930" yWindow="-16320" windowWidth="28110" windowHeight="16440" tabRatio="884" firstSheet="5" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AccessRight" sheetId="199" r:id="rId1"/>
@@ -308,7 +308,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="344">
   <si>
     <t>ListID</t>
   </si>
@@ -1198,39 +1198,15 @@
     <t>http://publications.europa.eu/resource/distribution/criterion/20210616-0/xml/gc/Criterion.gc</t>
   </si>
   <si>
-    <t>https://github.com/ESPD/ESPD-EDM/tree/v3.0.1</t>
-  </si>
-  <si>
     <t>20211208-0</t>
   </si>
   <si>
-    <t>https://github.com/ESPD/ESPD-EDM/tree/v3.0.1/codelists/gc/BooleanGUIControlType.gc</t>
-  </si>
-  <si>
-    <t>https://github.com/ESPD/ESPD-EDM/tree/v3.0.1/codelists/gc/CriterionElementType.gc</t>
-  </si>
-  <si>
     <t>http://publications.europa.eu/resource/dataset/eo-role-type/20211208-0</t>
   </si>
   <si>
     <t>http://publications.europa.eu/resource/distribution/eo-role-type/20211208-0/xml/gc/EoRoleType.gc</t>
   </si>
   <si>
-    <t>https://github.com/ESPD/ESPD-EDM/tree/v3.0.1/codelists/gc/FinancialRatioType.gc</t>
-  </si>
-  <si>
-    <t>https://github.com/ESPD/ESPD-EDM/tree/v3.0.1/codelists/gc/EOIDType.gc</t>
-  </si>
-  <si>
-    <t>https://github.com/ESPD/ESPD-EDM/tree/v3.0.1/codelists/gc/ProfileExecutionID.gc</t>
-  </si>
-  <si>
-    <t>https://github.com/ESPD/ESPD-EDM/tree/v3.0.1/codelists/gc/PropertyGroupType.gc</t>
-  </si>
-  <si>
-    <t>https://github.com/ESPD/ESPD-EDM/tree/v3.0.1/codelists/gc/ResponseDataType.gc</t>
-  </si>
-  <si>
     <t>CONFIDENTIAL</t>
   </si>
   <si>
@@ -1337,6 +1313,33 @@
   </si>
   <si>
     <t>3.1.0</t>
+  </si>
+  <si>
+    <t>https://github.com/ESPD/ESPD-EDM/tree/v3.1.0</t>
+  </si>
+  <si>
+    <t>https://github.com/ESPD/ESPD-EDM/tree/v3.1.0/codelists/gc/CriterionElementType.gc</t>
+  </si>
+  <si>
+    <t>https://github.com/OP-TED/ESPD-EDM/tree/3.1.0/</t>
+  </si>
+  <si>
+    <t>https://github.com/ESPD/ESPD-EDM/tree/v3.1.0/codelists/gc/BooleanGUIControlType.gc</t>
+  </si>
+  <si>
+    <t>https://github.com/ESPD/ESPD-EDM/tree/v3.1.0/codelists/gc/EOIDType.gc</t>
+  </si>
+  <si>
+    <t>https://github.com/ESPD/ESPD-EDM/tree/v3.1.0/codelists/gc/FinancialRatioType.gc</t>
+  </si>
+  <si>
+    <t>https://github.com/ESPD/ESPD-EDM/tree/v3.1.0/codelists/gc/ProfileExecutionID.gc</t>
+  </si>
+  <si>
+    <t>https://github.com/ESPD/ESPD-EDM/tree/v3.1.0/codelists/gc/PropertyGroupType.gc</t>
+  </si>
+  <si>
+    <t>https://github.com/ESPD/ESPD-EDM/tree/v3.1.0/codelists/gc/ResponseDataType.gc</t>
   </si>
 </sst>
 </file>
@@ -7125,7 +7128,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="C4" s="5"/>
     </row>
@@ -7143,7 +7146,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="C6" s="14"/>
       <c r="F6" s="21"/>
@@ -7153,7 +7156,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="C7" s="14"/>
     </row>
@@ -7263,42 +7266,42 @@
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="D11" t="s">
         <v>216</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="B12" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="D12" t="s">
         <v>216</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="L12" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.25">
@@ -7378,7 +7381,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="13" x14ac:dyDescent="0.3">
@@ -7394,7 +7397,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="13" x14ac:dyDescent="0.3">
@@ -7402,7 +7405,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="13" x14ac:dyDescent="0.3">
@@ -7439,7 +7442,7 @@
   <dimension ref="A1:AB38"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -7468,7 +7471,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
     </row>
     <row r="4" spans="1:28" ht="13" x14ac:dyDescent="0.3">
@@ -7484,7 +7487,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>296</v>
+        <v>335</v>
       </c>
     </row>
     <row r="6" spans="1:28" ht="13" x14ac:dyDescent="0.3">
@@ -7492,7 +7495,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>302</v>
+        <v>340</v>
       </c>
     </row>
     <row r="7" spans="1:28" ht="13" x14ac:dyDescent="0.3">
@@ -8504,7 +8507,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="C4" s="5"/>
     </row>
@@ -8522,7 +8525,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="C6" s="14"/>
     </row>
@@ -8531,7 +8534,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="C7" s="14"/>
     </row>
@@ -8603,7 +8606,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="C3" s="5"/>
     </row>
@@ -8612,7 +8615,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="C4" s="5"/>
     </row>
@@ -8621,7 +8624,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="C5" s="14"/>
     </row>
@@ -8630,7 +8633,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="C6" s="14"/>
     </row>
@@ -8639,7 +8642,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="C7" s="14"/>
     </row>
@@ -8648,7 +8651,7 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
@@ -8682,7 +8685,7 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
     </row>
   </sheetData>
@@ -8703,7 +8706,7 @@
   <dimension ref="A1:AB16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -8757,7 +8760,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>296</v>
+        <v>335</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -8767,7 +8770,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>304</v>
+        <v>341</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -9023,13 +9026,13 @@
     </row>
     <row r="16" spans="1:28" ht="16" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="D16" s="16" t="s">
         <v>216</v>
@@ -9042,7 +9045,7 @@
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
       <c r="L16" s="6" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="M16" s="6"/>
       <c r="N16" s="6"/>
@@ -9080,7 +9083,7 @@
   <dimension ref="A1:AB10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -9126,7 +9129,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>296</v>
+        <v>335</v>
       </c>
       <c r="C5" s="14"/>
     </row>
@@ -9135,7 +9138,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>305</v>
+        <v>342</v>
       </c>
       <c r="C6" s="14"/>
     </row>
@@ -9363,8 +9366,8 @@
   <sheetPr codeName="Hoja16"/>
   <dimension ref="A1:AB33"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -9417,7 +9420,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>296</v>
+        <v>335</v>
       </c>
       <c r="C5" s="17"/>
       <c r="D5" s="17"/>
@@ -9427,7 +9430,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>306</v>
+        <v>343</v>
       </c>
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>
@@ -9643,10 +9646,10 @@
         <v>12</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>216</v>
@@ -9659,7 +9662,7 @@
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
       <c r="L11" s="8" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="M11" s="8"/>
       <c r="N11" s="8"/>
@@ -10575,8 +10578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AB13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -10608,7 +10611,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="C3" s="5"/>
     </row>
@@ -10626,7 +10629,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>296</v>
+        <v>337</v>
       </c>
       <c r="C5" s="14"/>
     </row>
@@ -10635,7 +10638,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>298</v>
+        <v>338</v>
       </c>
       <c r="C6" s="14"/>
     </row>
@@ -11025,7 +11028,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="C4" s="5"/>
     </row>
@@ -11043,7 +11046,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="C6" s="1"/>
     </row>
@@ -11052,7 +11055,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="C7" s="1"/>
     </row>
@@ -11210,7 +11213,7 @@
   <dimension ref="A1:AB18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -11245,7 +11248,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -11265,7 +11268,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>296</v>
+        <v>335</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -11275,7 +11278,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>299</v>
+        <v>336</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -11822,7 +11825,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -11842,7 +11845,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -11852,7 +11855,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -11931,7 +11934,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -11941,7 +11944,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -11951,7 +11954,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -11961,7 +11964,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -11971,7 +11974,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -12055,7 +12058,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -12075,7 +12078,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -12085,7 +12088,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -12128,7 +12131,7 @@
   <dimension ref="A1:AB12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -12161,7 +12164,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -12181,7 +12184,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>296</v>
+        <v>335</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -12191,7 +12194,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>303</v>
+        <v>339</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -12496,21 +12499,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100087E4EC354ADFB40AC5D4FC129E379BA" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="29f822455ff5391d2c7c2dfd7717ecba">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="541a8a8b-b856-4d35-a5c7-7f2c0ec3d499" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="35e6952e7efa586d011e824f69a654f2" ns2:_="">
     <xsd:import namespace="541a8a8b-b856-4d35-a5c7-7f2c0ec3d499"/>
@@ -12682,10 +12670,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{742639C9-D5E0-4CBF-8139-6F41798C6819}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5774DC4B-7AB9-4854-9E79-56DDD4D64737}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="541a8a8b-b856-4d35-a5c7-7f2c0ec3d499"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -12707,19 +12720,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5774DC4B-7AB9-4854-9E79-56DDD4D64737}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{742639C9-D5E0-4CBF-8139-6F41798C6819}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="541a8a8b-b856-4d35-a5c7-7f2c0ec3d499"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
CL version bug fix
</commit_message>
<xml_diff>
--- a/__ESPDTeam__/ESPD-CodeLists.xlsx
+++ b/__ESPDTeam__/ESPD-CodeLists.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hricolor\Documents\GitHub\ESPD-EDM-3.1.0\__ESPDTeam__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8E76DE-301C-46D2-A2EE-AFDFB4E95C98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{419ECA5D-56F8-450B-BD7F-158BE5647017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="-16320" windowWidth="28110" windowHeight="16440" tabRatio="884" firstSheet="5" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24285" yWindow="3060" windowWidth="20910" windowHeight="11715" tabRatio="884" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AccessRight" sheetId="199" r:id="rId1"/>
@@ -308,7 +308,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="342">
   <si>
     <t>ListID</t>
   </si>
@@ -1147,9 +1147,6 @@
     <t>http://publications.europa.eu/resource/dataset/access-right</t>
   </si>
   <si>
-    <t>3.0.1</t>
-  </si>
-  <si>
     <t>http://publications.europa.eu/resource/authority/language</t>
   </si>
   <si>
@@ -1289,9 +1286,6 @@
   </si>
   <si>
     <t>EMPL</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 20220316-0</t>
   </si>
   <si>
     <t>http://publications.europa.eu/resource/dataset/access-right/20220316-0</t>
@@ -7091,7 +7085,7 @@
   <dimension ref="A1:AB17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -7128,7 +7122,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C4" s="5"/>
     </row>
@@ -7146,7 +7140,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C6" s="14"/>
       <c r="F6" s="21"/>
@@ -7156,7 +7150,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C7" s="14"/>
     </row>
@@ -7266,42 +7260,42 @@
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>298</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>299</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="C11" s="6" t="s">
         <v>300</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>301</v>
       </c>
       <c r="D11" t="s">
         <v>216</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>301</v>
+      </c>
+      <c r="B12" t="s">
         <v>302</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" s="6" t="s">
         <v>303</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>304</v>
       </c>
       <c r="D12" t="s">
         <v>216</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="L12" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.25">
@@ -7381,7 +7375,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="13" x14ac:dyDescent="0.3">
@@ -7397,7 +7391,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="13" x14ac:dyDescent="0.3">
@@ -7405,7 +7399,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="13" x14ac:dyDescent="0.3">
@@ -7463,7 +7457,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="3" spans="1:28" ht="13" x14ac:dyDescent="0.3">
@@ -7471,7 +7465,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="4" spans="1:28" ht="13" x14ac:dyDescent="0.3">
@@ -7487,7 +7481,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="6" spans="1:28" ht="13" x14ac:dyDescent="0.3">
@@ -7495,7 +7489,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="7" spans="1:28" ht="13" x14ac:dyDescent="0.3">
@@ -8499,7 +8493,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="13" x14ac:dyDescent="0.3">
@@ -8507,7 +8501,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C4" s="5"/>
     </row>
@@ -8516,7 +8510,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C5" s="14"/>
     </row>
@@ -8525,7 +8519,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C6" s="14"/>
     </row>
@@ -8534,7 +8528,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C7" s="14"/>
     </row>
@@ -8588,7 +8582,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C1" s="5"/>
     </row>
@@ -8606,7 +8600,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C3" s="5"/>
     </row>
@@ -8615,7 +8609,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C4" s="5"/>
     </row>
@@ -8624,7 +8618,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C5" s="14"/>
     </row>
@@ -8633,7 +8627,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C6" s="14"/>
     </row>
@@ -8642,7 +8636,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C7" s="14"/>
     </row>
@@ -8651,7 +8645,7 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
@@ -8685,7 +8679,7 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -8706,7 +8700,7 @@
   <dimension ref="A1:AB16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -8730,7 +8724,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -8740,7 +8734,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>279</v>
+        <v>332</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -8760,7 +8754,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -8770,7 +8764,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -9026,13 +9020,13 @@
     </row>
     <row r="16" spans="1:28" ht="16" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>307</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>307</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>308</v>
       </c>
       <c r="D16" s="16" t="s">
         <v>216</v>
@@ -9045,7 +9039,7 @@
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
       <c r="L16" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="M16" s="6"/>
       <c r="N16" s="6"/>
@@ -9083,7 +9077,7 @@
   <dimension ref="A1:AB10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -9102,7 +9096,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C2" s="5"/>
     </row>
@@ -9111,7 +9105,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>279</v>
+        <v>332</v>
       </c>
       <c r="C3" s="5"/>
     </row>
@@ -9129,7 +9123,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C5" s="14"/>
     </row>
@@ -9138,7 +9132,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C6" s="14"/>
     </row>
@@ -9366,8 +9360,8 @@
   <sheetPr codeName="Hoja16"/>
   <dimension ref="A1:AB33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -9390,7 +9384,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -9400,7 +9394,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>279</v>
+        <v>332</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -9420,7 +9414,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C5" s="17"/>
       <c r="D5" s="17"/>
@@ -9430,7 +9424,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>
@@ -9646,10 +9640,10 @@
         <v>12</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>216</v>
@@ -9662,7 +9656,7 @@
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
       <c r="L11" s="8" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="M11" s="8"/>
       <c r="N11" s="8"/>
@@ -10602,7 +10596,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C2" s="5"/>
     </row>
@@ -10611,7 +10605,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C3" s="5"/>
     </row>
@@ -10629,7 +10623,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C5" s="14"/>
     </row>
@@ -10638,7 +10632,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C6" s="14"/>
     </row>
@@ -11028,7 +11022,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C4" s="5"/>
     </row>
@@ -11046,7 +11040,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C6" s="1"/>
     </row>
@@ -11055,7 +11049,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C7" s="1"/>
     </row>
@@ -11094,7 +11088,7 @@
   <sheetPr codeName="Hoja5"/>
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -11129,7 +11123,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -11139,7 +11133,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -11149,7 +11143,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -11159,7 +11153,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="21"/>
@@ -11169,7 +11163,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -11238,7 +11232,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -11248,7 +11242,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -11268,7 +11262,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -11278,7 +11272,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -11825,7 +11819,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -11845,7 +11839,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -11855,7 +11849,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -11924,7 +11918,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -11934,7 +11928,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -11944,7 +11938,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -11954,7 +11948,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -11964,7 +11958,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -11974,7 +11968,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -12058,7 +12052,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -12078,7 +12072,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -12088,7 +12082,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -12154,7 +12148,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -12164,7 +12158,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -12184,7 +12178,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -12194,7 +12188,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -12499,6 +12493,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100087E4EC354ADFB40AC5D4FC129E379BA" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="29f822455ff5391d2c7c2dfd7717ecba">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="541a8a8b-b856-4d35-a5c7-7f2c0ec3d499" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="35e6952e7efa586d011e824f69a654f2" ns2:_="">
     <xsd:import namespace="541a8a8b-b856-4d35-a5c7-7f2c0ec3d499"/>
@@ -12670,35 +12679,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5774DC4B-7AB9-4854-9E79-56DDD4D64737}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{742639C9-D5E0-4CBF-8139-6F41798C6819}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="541a8a8b-b856-4d35-a5c7-7f2c0ec3d499"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -12720,9 +12704,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{742639C9-D5E0-4CBF-8139-6F41798C6819}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5774DC4B-7AB9-4854-9E79-56DDD4D64737}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="541a8a8b-b856-4d35-a5c7-7f2c0ec3d499"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Attributes update for all artefact alingment
</commit_message>
<xml_diff>
--- a/__ESPDTeam__/ESPD-CodeLists.xlsx
+++ b/__ESPDTeam__/ESPD-CodeLists.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25831"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hricolor\Documents\GitHub\ESPD-EDM-3.1.0\__ESPDTeam__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{419ECA5D-56F8-450B-BD7F-158BE5647017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E31C245-5566-4EEC-84A3-408D70ECAFE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24285" yWindow="3060" windowWidth="20910" windowHeight="11715" tabRatio="884" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27990" yWindow="-120" windowWidth="28110" windowHeight="16440" tabRatio="884" firstSheet="5" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AccessRight" sheetId="199" r:id="rId1"/>
@@ -308,7 +308,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="344">
   <si>
     <t>ListID</t>
   </si>
@@ -1334,6 +1334,12 @@
   </si>
   <si>
     <t>https://github.com/ESPD/ESPD-EDM/tree/v3.1.0/codelists/gc/ResponseDataType.gc</t>
+  </si>
+  <si>
+    <t>ESPD-EDMv3.1.0</t>
+  </si>
+  <si>
+    <t>European Single Procurement Document version 3.1.0</t>
   </si>
 </sst>
 </file>
@@ -6536,8 +6542,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF19000000}" name="Table7837136211455221705220992219922300224013" displayName="Table7837136211455221705220992219922300224013" ref="A7:AB16" tableType="xml" totalsRowShown="0" connectionId="66">
-  <autoFilter ref="A7:AB16" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF19000000}" name="Table7837136211455221705220992219922300224013" displayName="Table7837136211455221705220992219922300224013" ref="A7:AB17" tableType="xml" totalsRowShown="0" connectionId="66">
+  <autoFilter ref="A7:AB17" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A12:B41">
     <sortCondition ref="A12"/>
   </sortState>
@@ -8697,10 +8703,10 @@
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <sheetPr codeName="Hoja13"/>
-  <dimension ref="A1:AB16"/>
+  <dimension ref="A1:AB17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -9057,6 +9063,23 @@
       <c r="Z16" s="6"/>
       <c r="AA16" s="6"/>
       <c r="AB16" s="6"/>
+    </row>
+    <row r="17" spans="1:12" ht="16" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>342</v>
+      </c>
+      <c r="B17" t="s">
+        <v>342</v>
+      </c>
+      <c r="C17" t="s">
+        <v>343</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>216</v>
+      </c>
+      <c r="L17" t="s">
+        <v>342</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -11088,7 +11111,7 @@
   <sheetPr codeName="Hoja5"/>
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -12493,21 +12516,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100087E4EC354ADFB40AC5D4FC129E379BA" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="29f822455ff5391d2c7c2dfd7717ecba">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="541a8a8b-b856-4d35-a5c7-7f2c0ec3d499" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="35e6952e7efa586d011e824f69a654f2" ns2:_="">
     <xsd:import namespace="541a8a8b-b856-4d35-a5c7-7f2c0ec3d499"/>
@@ -12679,15 +12693,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{742639C9-D5E0-4CBF-8139-6F41798C6819}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E61FB905-6753-4D6B-9555-45A818BB6BAA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="541a8a8b-b856-4d35-a5c7-7f2c0ec3d499"/>
@@ -12703,7 +12718,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5774DC4B-7AB9-4854-9E79-56DDD4D64737}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12719,4 +12734,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{742639C9-D5E0-4CBF-8139-6F41798C6819}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
ResponseDataTypes fixes for ESPD-EDMv3.1.0
</commit_message>
<xml_diff>
--- a/__ESPDTeam__/ESPD-CodeLists.xlsx
+++ b/__ESPDTeam__/ESPD-CodeLists.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hricolor\Documents\GitHub\ESPD-EDM-3.1.0\__ESPDTeam__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E31C245-5566-4EEC-84A3-408D70ECAFE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBF7220F-E76B-41F8-86B6-460D71741860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27990" yWindow="-120" windowWidth="28110" windowHeight="16440" tabRatio="884" firstSheet="5" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21240" yWindow="675" windowWidth="20910" windowHeight="11715" tabRatio="884" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AccessRight" sheetId="199" r:id="rId1"/>
@@ -8705,7 +8705,7 @@
   <sheetPr codeName="Hoja13"/>
   <dimension ref="A1:AB17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -10595,8 +10595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AB13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -12516,9 +12516,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -12694,26 +12697,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E61FB905-6753-4D6B-9555-45A818BB6BAA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{742639C9-D5E0-4CBF-8139-6F41798C6819}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="541a8a8b-b856-4d35-a5c7-7f2c0ec3d499"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -12737,9 +12729,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{742639C9-D5E0-4CBF-8139-6F41798C6819}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E61FB905-6753-4D6B-9555-45A818BB6BAA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="541a8a8b-b856-4d35-a5c7-7f2c0ec3d499"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fix to github issue #325  , subtask TEDSPD-489
</commit_message>
<xml_diff>
--- a/__ESPDTeam__/ESPD-CodeLists.xlsx
+++ b/__ESPDTeam__/ESPD-CodeLists.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25928"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hricolor\Documents\GitHub\ESPD-EDM-3.1.0\__ESPDTeam__\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\JC\Proyectos\17 - OP - ESPD\ESPD-EDM\__ESPDTeam__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBF7220F-E76B-41F8-86B6-460D71741860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49A3D0F7-A9C9-4254-B064-06443654BF70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21240" yWindow="675" windowWidth="20910" windowHeight="11715" tabRatio="884" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="884" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AccessRight" sheetId="199" r:id="rId1"/>
@@ -48,7 +48,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>ARILLO ARANDA Paloma (OP):</t>
         </r>
@@ -57,7 +57,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Descriptions to be revised, see R22 for example</t>
@@ -1186,15 +1186,6 @@
     <t>financial-ratio-type</t>
   </si>
   <si>
-    <t>20210616-0</t>
-  </si>
-  <si>
-    <t>http://publications.europa.eu/resource/dataset/criterion/20210616-0</t>
-  </si>
-  <si>
-    <t>http://publications.europa.eu/resource/distribution/criterion/20210616-0/xml/gc/Criterion.gc</t>
-  </si>
-  <si>
     <t>20211208-0</t>
   </si>
   <si>
@@ -1340,6 +1331,15 @@
   </si>
   <si>
     <t>European Single Procurement Document version 3.1.0</t>
+  </si>
+  <si>
+    <t>20230118-0</t>
+  </si>
+  <si>
+    <t>http://publications.europa.eu/resource/dataset/criterion/20230118-0</t>
+  </si>
+  <si>
+    <t>http://publications.europa.eu/resource/distribution/criterion/20230118-0/xml/gc/Criterion.gc</t>
   </si>
 </sst>
 </file>
@@ -1432,14 +1432,14 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -7094,9 +7094,9 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -7105,7 +7105,7 @@
       </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -7114,7 +7114,7 @@
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -7123,16 +7123,16 @@
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -7141,26 +7141,26 @@
       </c>
       <c r="C5" s="14"/>
     </row>
-    <row r="6" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C6" s="14"/>
       <c r="F6" s="21"/>
     </row>
-    <row r="7" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C7" s="14"/>
     </row>
-    <row r="8" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -7169,7 +7169,7 @@
       </c>
       <c r="C8" s="5"/>
     </row>
-    <row r="9" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -7178,7 +7178,7 @@
       </c>
       <c r="C9" s="5"/>
     </row>
-    <row r="10" spans="1:28" ht="16.5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:28" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -7266,58 +7266,58 @@
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="D11" t="s">
         <v>216</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B12" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D12" t="s">
         <v>216</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="L12" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C13" s="6"/>
       <c r="J13" s="6"/>
     </row>
-    <row r="14" spans="1:28" ht="16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" ht="15" x14ac:dyDescent="0.25">
       <c r="D14" s="16"/>
     </row>
-    <row r="15" spans="1:28" ht="16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" ht="15" x14ac:dyDescent="0.25">
       <c r="D15" s="16"/>
     </row>
-    <row r="16" spans="1:28" ht="16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" ht="15" x14ac:dyDescent="0.25">
       <c r="D16" s="16"/>
     </row>
-    <row r="17" spans="4:4" ht="16" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:4" ht="15" x14ac:dyDescent="0.25">
       <c r="D17" s="16"/>
     </row>
   </sheetData>
@@ -7344,15 +7344,15 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.36328125" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="33.54296875" customWidth="1"/>
-    <col min="4" max="4" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.5546875" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -7360,7 +7360,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -7368,7 +7368,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -7376,15 +7376,15 @@
         <v>272</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -7392,23 +7392,23 @@
         <v>271</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -7416,7 +7416,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -7445,12 +7445,12 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -7458,7 +7458,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -7466,15 +7466,15 @@
         <v>291</v>
       </c>
     </row>
-    <row r="3" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="4" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -7482,23 +7482,23 @@
         <v>203</v>
       </c>
     </row>
-    <row r="5" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="6" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="7" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
@@ -7506,7 +7506,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
@@ -7514,7 +7514,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:28" ht="16.5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:28" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -8470,13 +8470,13 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.90625" customWidth="1"/>
-    <col min="4" max="4" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.88671875" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -8485,7 +8485,7 @@
       </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -8494,7 +8494,7 @@
       </c>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -8502,16 +8502,16 @@
         <v>279</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -8520,25 +8520,25 @@
       </c>
       <c r="C5" s="14"/>
     </row>
-    <row r="6" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C6" s="14"/>
     </row>
-    <row r="7" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C7" s="14"/>
     </row>
-    <row r="8" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -8547,7 +8547,7 @@
       </c>
       <c r="C8" s="5"/>
     </row>
-    <row r="9" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -8576,14 +8576,14 @@
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.90625" customWidth="1"/>
-    <col min="2" max="2" width="22.453125" customWidth="1"/>
-    <col min="3" max="3" width="18.54296875" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" customWidth="1"/>
+    <col min="2" max="2" width="22.44140625" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -8592,7 +8592,7 @@
       </c>
       <c r="C1" s="5"/>
     </row>
-    <row r="2" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -8601,57 +8601,57 @@
       </c>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C5" s="14"/>
     </row>
-    <row r="6" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C6" s="14"/>
     </row>
-    <row r="7" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C7" s="14"/>
     </row>
-    <row r="8" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
@@ -8680,12 +8680,12 @@
       <c r="AA8" s="6"/>
       <c r="AB8" s="6"/>
     </row>
-    <row r="9" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
   </sheetData>
@@ -8709,13 +8709,13 @@
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.453125" customWidth="1"/>
+    <col min="1" max="1" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -8725,7 +8725,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -8735,17 +8735,17 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -8755,27 +8755,27 @@
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
     </row>
-    <row r="5" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
     </row>
-    <row r="6" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
     </row>
-    <row r="7" spans="1:28" ht="16.5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:28" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
         <v>8</v>
       </c>
@@ -8896,7 +8896,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="10" spans="1:28" ht="16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>242</v>
       </c>
@@ -8913,7 +8913,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="11" spans="1:28" ht="16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>243</v>
       </c>
@@ -8931,7 +8931,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="12" spans="1:28" ht="16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>212</v>
       </c>
@@ -8948,7 +8948,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="13" spans="1:28" ht="16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>246</v>
       </c>
@@ -8967,7 +8967,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="14" spans="1:28" ht="16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>249</v>
       </c>
@@ -8984,7 +8984,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="15" spans="1:28" ht="16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>250</v>
       </c>
@@ -9024,15 +9024,15 @@
       <c r="AA15" s="6"/>
       <c r="AB15" s="6"/>
     </row>
-    <row r="16" spans="1:28" ht="16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D16" s="16" t="s">
         <v>216</v>
@@ -9045,7 +9045,7 @@
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
       <c r="L16" s="6" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="M16" s="6"/>
       <c r="N16" s="6"/>
@@ -9064,21 +9064,21 @@
       <c r="AA16" s="6"/>
       <c r="AB16" s="6"/>
     </row>
-    <row r="17" spans="1:12" ht="16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="B17" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="C17" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D17" s="16" t="s">
         <v>216</v>
       </c>
       <c r="L17" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
   </sheetData>
@@ -9103,9 +9103,9 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -9114,7 +9114,7 @@
       </c>
       <c r="C1" s="5"/>
     </row>
-    <row r="2" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -9123,16 +9123,16 @@
       </c>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -9141,25 +9141,25 @@
       </c>
       <c r="C4" s="14"/>
     </row>
-    <row r="5" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="C5" s="14"/>
     </row>
-    <row r="6" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="C6" s="14"/>
     </row>
-    <row r="7" spans="1:28" ht="16.5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:28" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -9387,12 +9387,12 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.36328125" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.33203125" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>5</v>
       </c>
@@ -9402,7 +9402,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
@@ -9412,17 +9412,17 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -9432,27 +9432,27 @@
       <c r="C4" s="17"/>
       <c r="D4" s="17"/>
     </row>
-    <row r="5" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="C5" s="17"/>
       <c r="D5" s="17"/>
     </row>
-    <row r="6" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>
     </row>
-    <row r="7" spans="1:28" ht="16.5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:28" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
         <v>8</v>
       </c>
@@ -9663,10 +9663,10 @@
         <v>12</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>216</v>
@@ -9679,7 +9679,7 @@
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
       <c r="L11" s="8" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="M11" s="8"/>
       <c r="N11" s="8"/>
@@ -10595,17 +10595,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AB13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.90625" customWidth="1"/>
-    <col min="2" max="2" width="22.453125" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" customWidth="1"/>
+    <col min="2" max="2" width="22.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -10614,7 +10614,7 @@
       </c>
       <c r="C1" s="5"/>
     </row>
-    <row r="2" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -10623,16 +10623,16 @@
       </c>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -10641,25 +10641,25 @@
       </c>
       <c r="C4" s="14"/>
     </row>
-    <row r="5" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="C5" s="14"/>
     </row>
-    <row r="6" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="C6" s="14"/>
     </row>
-    <row r="7" spans="1:28" ht="16.5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:28" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -11008,12 +11008,12 @@
       <selection activeCell="A8" sqref="A8:A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -11022,7 +11022,7 @@
       </c>
       <c r="C1" s="5"/>
     </row>
-    <row r="2" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -11031,7 +11031,7 @@
       </c>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -11040,16 +11040,16 @@
       </c>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -11058,25 +11058,25 @@
       </c>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -11085,7 +11085,7 @@
       </c>
       <c r="C8" s="5"/>
     </row>
-    <row r="9" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -11111,17 +11111,17 @@
   <sheetPr codeName="Hoja5"/>
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.453125" customWidth="1"/>
-    <col min="2" max="2" width="40.08984375" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" customWidth="1"/>
+    <col min="2" max="2" width="40.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -11131,7 +11131,7 @@
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
     </row>
-    <row r="2" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -11141,7 +11141,7 @@
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
     </row>
-    <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -11151,17 +11151,17 @@
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>292</v>
+        <v>341</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -11171,27 +11171,27 @@
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
     </row>
-    <row r="6" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>293</v>
+        <v>342</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="21"/>
     </row>
-    <row r="7" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>294</v>
+        <v>343</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
     </row>
-    <row r="8" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -11201,7 +11201,7 @@
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
     </row>
-    <row r="9" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -11233,14 +11233,14 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.08984375" customWidth="1"/>
-    <col min="2" max="2" width="30.54296875" customWidth="1"/>
-    <col min="4" max="4" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.109375" customWidth="1"/>
+    <col min="2" max="2" width="30.5546875" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -11250,7 +11250,7 @@
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
     </row>
-    <row r="2" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -11260,17 +11260,17 @@
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
     </row>
-    <row r="3" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -11280,27 +11280,27 @@
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
     </row>
-    <row r="5" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
     </row>
-    <row r="6" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
     </row>
-    <row r="7" spans="1:28" ht="16.5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:28" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -11802,12 +11802,12 @@
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.54296875" customWidth="1"/>
+    <col min="1" max="1" width="21.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -11817,7 +11817,7 @@
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
     </row>
-    <row r="2" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -11827,7 +11827,7 @@
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
     </row>
-    <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -11837,17 +11837,17 @@
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -11857,27 +11857,27 @@
       <c r="C5" s="15"/>
       <c r="D5" s="15"/>
     </row>
-    <row r="6" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
     </row>
-    <row r="7" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
     </row>
-    <row r="8" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -11887,7 +11887,7 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -11918,15 +11918,15 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.90625" customWidth="1"/>
-    <col min="2" max="2" width="26.08984375" customWidth="1"/>
-    <col min="3" max="3" width="24.54296875" customWidth="1"/>
-    <col min="4" max="4" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" customWidth="1"/>
+    <col min="2" max="2" width="26.109375" customWidth="1"/>
+    <col min="3" max="3" width="24.5546875" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -11936,7 +11936,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -11946,57 +11946,57 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
     </row>
-    <row r="6" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
     </row>
-    <row r="7" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
     </row>
-    <row r="8" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -12004,7 +12004,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -12033,14 +12033,14 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="2" width="21.08984375" customWidth="1"/>
-    <col min="4" max="4" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.109375" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -12050,7 +12050,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -12060,7 +12060,7 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -12070,17 +12070,17 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -12090,27 +12090,27 @@
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
     </row>
-    <row r="6" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
     </row>
-    <row r="7" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
     </row>
-    <row r="8" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -12120,7 +12120,7 @@
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
     </row>
-    <row r="9" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -12151,12 +12151,12 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -12166,7 +12166,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -12176,17 +12176,17 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -12196,27 +12196,27 @@
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
     </row>
-    <row r="5" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
     </row>
-    <row r="6" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
     </row>
-    <row r="7" spans="1:28" ht="16.5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:28" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -12525,6 +12525,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100087E4EC354ADFB40AC5D4FC129E379BA" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="29f822455ff5391d2c7c2dfd7717ecba">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="541a8a8b-b856-4d35-a5c7-7f2c0ec3d499" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="35e6952e7efa586d011e824f69a654f2" ns2:_="">
     <xsd:import namespace="541a8a8b-b856-4d35-a5c7-7f2c0ec3d499"/>
@@ -12696,12 +12702,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{742639C9-D5E0-4CBF-8139-6F41798C6819}">
   <ds:schemaRefs>
@@ -12711,6 +12711,22 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E61FB905-6753-4D6B-9555-45A818BB6BAA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="541a8a8b-b856-4d35-a5c7-7f2c0ec3d499"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5774DC4B-7AB9-4854-9E79-56DDD4D64737}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12726,20 +12742,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E61FB905-6753-4D6B-9555-45A818BB6BAA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="541a8a8b-b856-4d35-a5c7-7f2c0ec3d499"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Revert "Fix to github issue #325  , subtask TEDSPD-489"
This reverts commit 04b53e7bded3a5ee6d44511ca7bc7369658b8340.
</commit_message>
<xml_diff>
--- a/__ESPDTeam__/ESPD-CodeLists.xlsx
+++ b/__ESPDTeam__/ESPD-CodeLists.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25831"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\JC\Proyectos\17 - OP - ESPD\ESPD-EDM\__ESPDTeam__\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hricolor\Documents\GitHub\ESPD-EDM-3.1.0\__ESPDTeam__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49A3D0F7-A9C9-4254-B064-06443654BF70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBF7220F-E76B-41F8-86B6-460D71741860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="884" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21240" yWindow="675" windowWidth="20910" windowHeight="11715" tabRatio="884" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AccessRight" sheetId="199" r:id="rId1"/>
@@ -48,7 +48,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t>ARILLO ARANDA Paloma (OP):</t>
         </r>
@@ -57,7 +57,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
 Descriptions to be revised, see R22 for example</t>
@@ -1186,6 +1186,15 @@
     <t>financial-ratio-type</t>
   </si>
   <si>
+    <t>20210616-0</t>
+  </si>
+  <si>
+    <t>http://publications.europa.eu/resource/dataset/criterion/20210616-0</t>
+  </si>
+  <si>
+    <t>http://publications.europa.eu/resource/distribution/criterion/20210616-0/xml/gc/Criterion.gc</t>
+  </si>
+  <si>
     <t>20211208-0</t>
   </si>
   <si>
@@ -1331,15 +1340,6 @@
   </si>
   <si>
     <t>European Single Procurement Document version 3.1.0</t>
-  </si>
-  <si>
-    <t>20230118-0</t>
-  </si>
-  <si>
-    <t>http://publications.europa.eu/resource/dataset/criterion/20230118-0</t>
-  </si>
-  <si>
-    <t>http://publications.europa.eu/resource/distribution/criterion/20230118-0/xml/gc/Criterion.gc</t>
   </si>
 </sst>
 </file>
@@ -1432,14 +1432,14 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="9"/>
@@ -7094,9 +7094,9 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -7105,7 +7105,7 @@
       </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -7114,7 +7114,7 @@
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -7123,16 +7123,16 @@
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -7141,26 +7141,26 @@
       </c>
       <c r="C5" s="14"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="C6" s="14"/>
       <c r="F6" s="21"/>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="C7" s="14"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -7169,7 +7169,7 @@
       </c>
       <c r="C8" s="5"/>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -7178,7 +7178,7 @@
       </c>
       <c r="C9" s="5"/>
     </row>
-    <row r="10" spans="1:28" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:28" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -7266,58 +7266,58 @@
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="D11" t="s">
         <v>216</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="B12" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="D12" t="s">
         <v>216</v>
       </c>
       <c r="J12" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="L12" t="s">
         <v>302</v>
-      </c>
-      <c r="L12" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C13" s="6"/>
       <c r="J13" s="6"/>
     </row>
-    <row r="14" spans="1:28" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" ht="16" x14ac:dyDescent="0.25">
       <c r="D14" s="16"/>
     </row>
-    <row r="15" spans="1:28" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" ht="16" x14ac:dyDescent="0.25">
       <c r="D15" s="16"/>
     </row>
-    <row r="16" spans="1:28" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" ht="16" x14ac:dyDescent="0.25">
       <c r="D16" s="16"/>
     </row>
-    <row r="17" spans="4:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:4" ht="16" x14ac:dyDescent="0.25">
       <c r="D17" s="16"/>
     </row>
   </sheetData>
@@ -7344,15 +7344,15 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" customWidth="1"/>
+    <col min="1" max="1" width="23.36328125" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="33.5546875" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.54296875" customWidth="1"/>
+    <col min="4" max="4" width="8.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -7360,7 +7360,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -7368,7 +7368,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -7376,15 +7376,15 @@
         <v>272</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="13" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -7392,23 +7392,23 @@
         <v>271</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="13" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="13" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="13" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -7416,7 +7416,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="13" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -7445,12 +7445,12 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -7458,7 +7458,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -7466,15 +7466,15 @@
         <v>291</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -7482,23 +7482,23 @@
         <v>203</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
@@ -7506,7 +7506,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
@@ -7514,7 +7514,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:28" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:28" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -8470,13 +8470,13 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.90625" customWidth="1"/>
+    <col min="4" max="4" width="8.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -8485,7 +8485,7 @@
       </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -8494,7 +8494,7 @@
       </c>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -8502,16 +8502,16 @@
         <v>279</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -8520,25 +8520,25 @@
       </c>
       <c r="C5" s="14"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="C6" s="14"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="C7" s="14"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -8547,7 +8547,7 @@
       </c>
       <c r="C8" s="5"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -8576,14 +8576,14 @@
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" customWidth="1"/>
-    <col min="2" max="2" width="22.44140625" customWidth="1"/>
-    <col min="3" max="3" width="18.5546875" customWidth="1"/>
+    <col min="1" max="1" width="19.90625" customWidth="1"/>
+    <col min="2" max="2" width="22.453125" customWidth="1"/>
+    <col min="3" max="3" width="18.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -8592,7 +8592,7 @@
       </c>
       <c r="C1" s="5"/>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -8601,57 +8601,57 @@
       </c>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="C5" s="14"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="C6" s="14"/>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="C7" s="14"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
@@ -8680,12 +8680,12 @@
       <c r="AA8" s="6"/>
       <c r="AB8" s="6"/>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -8709,13 +8709,13 @@
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.44140625" customWidth="1"/>
+    <col min="1" max="1" width="27.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -8725,7 +8725,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -8735,17 +8735,17 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -8755,27 +8755,27 @@
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
     </row>
-    <row r="7" spans="1:28" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:28" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A7" s="8" t="s">
         <v>8</v>
       </c>
@@ -8896,7 +8896,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="10" spans="1:28" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" ht="16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>242</v>
       </c>
@@ -8913,7 +8913,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="11" spans="1:28" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" ht="16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>243</v>
       </c>
@@ -8931,7 +8931,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="12" spans="1:28" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" ht="16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>212</v>
       </c>
@@ -8948,7 +8948,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="13" spans="1:28" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" ht="16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>246</v>
       </c>
@@ -8967,7 +8967,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="14" spans="1:28" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" ht="16" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>249</v>
       </c>
@@ -8984,7 +8984,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="15" spans="1:28" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" ht="16" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>250</v>
       </c>
@@ -9024,15 +9024,15 @@
       <c r="AA15" s="6"/>
       <c r="AB15" s="6"/>
     </row>
-    <row r="16" spans="1:28" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" ht="16" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="D16" s="16" t="s">
         <v>216</v>
@@ -9045,7 +9045,7 @@
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
       <c r="L16" s="6" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="M16" s="6"/>
       <c r="N16" s="6"/>
@@ -9064,21 +9064,21 @@
       <c r="AA16" s="6"/>
       <c r="AB16" s="6"/>
     </row>
-    <row r="17" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="B17" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="C17" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="D17" s="16" t="s">
         <v>216</v>
       </c>
       <c r="L17" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
     </row>
   </sheetData>
@@ -9103,9 +9103,9 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -9114,7 +9114,7 @@
       </c>
       <c r="C1" s="5"/>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -9123,16 +9123,16 @@
       </c>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -9141,25 +9141,25 @@
       </c>
       <c r="C4" s="14"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="C5" s="14"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="C6" s="14"/>
     </row>
-    <row r="7" spans="1:28" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:28" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -9387,12 +9387,12 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.36328125" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>5</v>
       </c>
@@ -9402,7 +9402,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
@@ -9412,17 +9412,17 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -9432,27 +9432,27 @@
       <c r="C4" s="17"/>
       <c r="D4" s="17"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="C5" s="17"/>
       <c r="D5" s="17"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>
     </row>
-    <row r="7" spans="1:28" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:28" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A7" s="8" t="s">
         <v>8</v>
       </c>
@@ -9663,10 +9663,10 @@
         <v>12</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>216</v>
@@ -9679,7 +9679,7 @@
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
       <c r="L11" s="8" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="M11" s="8"/>
       <c r="N11" s="8"/>
@@ -10595,17 +10595,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AB13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" customWidth="1"/>
-    <col min="2" max="2" width="22.44140625" customWidth="1"/>
+    <col min="1" max="1" width="19.90625" customWidth="1"/>
+    <col min="2" max="2" width="22.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -10614,7 +10614,7 @@
       </c>
       <c r="C1" s="5"/>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -10623,16 +10623,16 @@
       </c>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -10641,25 +10641,25 @@
       </c>
       <c r="C4" s="14"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="C5" s="14"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="C6" s="14"/>
     </row>
-    <row r="7" spans="1:28" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:28" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -11008,12 +11008,12 @@
       <selection activeCell="A8" sqref="A8:A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -11022,7 +11022,7 @@
       </c>
       <c r="C1" s="5"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -11031,7 +11031,7 @@
       </c>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -11040,16 +11040,16 @@
       </c>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -11058,25 +11058,25 @@
       </c>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -11085,7 +11085,7 @@
       </c>
       <c r="C8" s="5"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -11111,17 +11111,17 @@
   <sheetPr codeName="Hoja5"/>
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.44140625" customWidth="1"/>
-    <col min="2" max="2" width="40.109375" customWidth="1"/>
+    <col min="1" max="1" width="19.453125" customWidth="1"/>
+    <col min="2" max="2" width="40.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -11131,7 +11131,7 @@
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -11141,7 +11141,7 @@
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -11151,17 +11151,17 @@
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>341</v>
+        <v>292</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -11171,27 +11171,27 @@
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>342</v>
+        <v>293</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="21"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>343</v>
+        <v>294</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -11201,7 +11201,7 @@
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -11233,14 +11233,14 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.109375" customWidth="1"/>
-    <col min="2" max="2" width="30.5546875" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.08984375" customWidth="1"/>
+    <col min="2" max="2" width="30.54296875" customWidth="1"/>
+    <col min="4" max="4" width="8.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -11250,7 +11250,7 @@
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -11260,17 +11260,17 @@
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -11280,27 +11280,27 @@
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
     </row>
-    <row r="7" spans="1:28" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:28" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -11802,12 +11802,12 @@
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5546875" customWidth="1"/>
+    <col min="1" max="1" width="21.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -11817,7 +11817,7 @@
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -11827,7 +11827,7 @@
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -11837,17 +11837,17 @@
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -11857,27 +11857,27 @@
       <c r="C5" s="15"/>
       <c r="D5" s="15"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -11887,7 +11887,7 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -11918,15 +11918,15 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" customWidth="1"/>
-    <col min="2" max="2" width="26.109375" customWidth="1"/>
-    <col min="3" max="3" width="24.5546875" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.90625" customWidth="1"/>
+    <col min="2" max="2" width="26.08984375" customWidth="1"/>
+    <col min="3" max="3" width="24.54296875" customWidth="1"/>
+    <col min="4" max="4" width="8.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -11936,7 +11936,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -11946,57 +11946,57 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -12004,7 +12004,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -12033,14 +12033,14 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="2" width="21.109375" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.08984375" customWidth="1"/>
+    <col min="4" max="4" width="8.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -12050,7 +12050,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -12060,7 +12060,7 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -12070,17 +12070,17 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -12090,27 +12090,27 @@
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -12120,7 +12120,7 @@
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -12151,12 +12151,12 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -12166,7 +12166,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -12176,17 +12176,17 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -12196,27 +12196,27 @@
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
     </row>
-    <row r="7" spans="1:28" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:28" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -12525,12 +12525,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100087E4EC354ADFB40AC5D4FC129E379BA" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="29f822455ff5391d2c7c2dfd7717ecba">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="541a8a8b-b856-4d35-a5c7-7f2c0ec3d499" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="35e6952e7efa586d011e824f69a654f2" ns2:_="">
     <xsd:import namespace="541a8a8b-b856-4d35-a5c7-7f2c0ec3d499"/>
@@ -12702,6 +12696,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{742639C9-D5E0-4CBF-8139-6F41798C6819}">
   <ds:schemaRefs>
@@ -12711,22 +12711,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E61FB905-6753-4D6B-9555-45A818BB6BAA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="541a8a8b-b856-4d35-a5c7-7f2c0ec3d499"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5774DC4B-7AB9-4854-9E79-56DDD4D64737}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12742,4 +12726,20 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E61FB905-6753-4D6B-9555-45A818BB6BAA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="541a8a8b-b856-4d35-a5c7-7f2c0ec3d499"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated version in technical codelists for 3.2.0 release
</commit_message>
<xml_diff>
--- a/__ESPDTeam__/ESPD-CodeLists.xlsx
+++ b/__ESPDTeam__/ESPD-CodeLists.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hricolor\Documents\GitHub\ESPD-EDM-3.1.0\__ESPDTeam__\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\JC\Proyectos\17 - OP - ESPD\ESPD-EDM\__ESPDTeam__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBF7220F-E76B-41F8-86B6-460D71741860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD7B995D-B373-46EA-B8BD-EC29B48D6AF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21240" yWindow="675" windowWidth="20910" windowHeight="11715" tabRatio="884" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="884" firstSheet="7" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AccessRight" sheetId="199" r:id="rId1"/>
@@ -1306,9 +1306,6 @@
     <t>http://publications.europa.eu/resource/authority/occupation</t>
   </si>
   <si>
-    <t>3.1.0</t>
-  </si>
-  <si>
     <t>https://github.com/ESPD/ESPD-EDM/tree/v3.1.0</t>
   </si>
   <si>
@@ -1340,6 +1337,9 @@
   </si>
   <si>
     <t>European Single Procurement Document version 3.1.0</t>
+  </si>
+  <si>
+    <t>3.2.0</t>
   </si>
 </sst>
 </file>
@@ -7094,9 +7094,9 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -7105,7 +7105,7 @@
       </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -7114,7 +7114,7 @@
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -7123,7 +7123,7 @@
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -7132,7 +7132,7 @@
       </c>
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -7141,7 +7141,7 @@
       </c>
       <c r="C5" s="14"/>
     </row>
-    <row r="6" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -7151,7 +7151,7 @@
       <c r="C6" s="14"/>
       <c r="F6" s="21"/>
     </row>
-    <row r="7" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -7160,7 +7160,7 @@
       </c>
       <c r="C7" s="14"/>
     </row>
-    <row r="8" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -7169,7 +7169,7 @@
       </c>
       <c r="C8" s="5"/>
     </row>
-    <row r="9" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -7178,7 +7178,7 @@
       </c>
       <c r="C9" s="5"/>
     </row>
-    <row r="10" spans="1:28" ht="16.5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:28" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -7308,16 +7308,16 @@
       <c r="C13" s="6"/>
       <c r="J13" s="6"/>
     </row>
-    <row r="14" spans="1:28" ht="16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" ht="15" x14ac:dyDescent="0.25">
       <c r="D14" s="16"/>
     </row>
-    <row r="15" spans="1:28" ht="16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" ht="15" x14ac:dyDescent="0.25">
       <c r="D15" s="16"/>
     </row>
-    <row r="16" spans="1:28" ht="16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" ht="15" x14ac:dyDescent="0.25">
       <c r="D16" s="16"/>
     </row>
-    <row r="17" spans="4:4" ht="16" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:4" ht="15" x14ac:dyDescent="0.25">
       <c r="D17" s="16"/>
     </row>
   </sheetData>
@@ -7344,15 +7344,15 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.36328125" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="33.54296875" customWidth="1"/>
-    <col min="4" max="4" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.5546875" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -7360,7 +7360,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -7368,7 +7368,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -7376,7 +7376,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -7384,7 +7384,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -7392,7 +7392,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -7400,7 +7400,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -7408,7 +7408,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -7416,7 +7416,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -7442,15 +7442,15 @@
   <dimension ref="A1:AB38"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -7458,7 +7458,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -7466,15 +7466,15 @@
         <v>291</v>
       </c>
     </row>
-    <row r="3" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="4" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -7482,23 +7482,23 @@
         <v>203</v>
       </c>
     </row>
-    <row r="5" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="6" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="7" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
@@ -7506,7 +7506,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
@@ -7514,7 +7514,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:28" ht="16.5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:28" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -8470,13 +8470,13 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.90625" customWidth="1"/>
-    <col min="4" max="4" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.88671875" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -8485,7 +8485,7 @@
       </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -8494,7 +8494,7 @@
       </c>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -8502,7 +8502,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -8511,7 +8511,7 @@
       </c>
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -8520,7 +8520,7 @@
       </c>
       <c r="C5" s="14"/>
     </row>
-    <row r="6" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -8529,7 +8529,7 @@
       </c>
       <c r="C6" s="14"/>
     </row>
-    <row r="7" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -8538,7 +8538,7 @@
       </c>
       <c r="C7" s="14"/>
     </row>
-    <row r="8" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -8547,7 +8547,7 @@
       </c>
       <c r="C8" s="5"/>
     </row>
-    <row r="9" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -8576,14 +8576,14 @@
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.90625" customWidth="1"/>
-    <col min="2" max="2" width="22.453125" customWidth="1"/>
-    <col min="3" max="3" width="18.54296875" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" customWidth="1"/>
+    <col min="2" max="2" width="22.44140625" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -8592,7 +8592,7 @@
       </c>
       <c r="C1" s="5"/>
     </row>
-    <row r="2" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -8601,7 +8601,7 @@
       </c>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -8610,7 +8610,7 @@
       </c>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -8619,7 +8619,7 @@
       </c>
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -8628,7 +8628,7 @@
       </c>
       <c r="C5" s="14"/>
     </row>
-    <row r="6" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -8637,7 +8637,7 @@
       </c>
       <c r="C6" s="14"/>
     </row>
-    <row r="7" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -8646,7 +8646,7 @@
       </c>
       <c r="C7" s="14"/>
     </row>
-    <row r="8" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -8680,7 +8680,7 @@
       <c r="AA8" s="6"/>
       <c r="AB8" s="6"/>
     </row>
-    <row r="9" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -8706,16 +8706,16 @@
   <dimension ref="A1:AB17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.453125" customWidth="1"/>
+    <col min="1" max="1" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -8725,7 +8725,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -8735,17 +8735,17 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>332</v>
+        <v>343</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -8755,27 +8755,27 @@
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
     </row>
-    <row r="5" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
     </row>
-    <row r="6" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
     </row>
-    <row r="7" spans="1:28" ht="16.5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:28" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
         <v>8</v>
       </c>
@@ -8896,7 +8896,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="10" spans="1:28" ht="16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>242</v>
       </c>
@@ -8913,7 +8913,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="11" spans="1:28" ht="16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>243</v>
       </c>
@@ -8931,7 +8931,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="12" spans="1:28" ht="16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>212</v>
       </c>
@@ -8948,7 +8948,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="13" spans="1:28" ht="16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>246</v>
       </c>
@@ -8967,7 +8967,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="14" spans="1:28" ht="16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>249</v>
       </c>
@@ -8984,7 +8984,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="15" spans="1:28" ht="16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>250</v>
       </c>
@@ -9024,7 +9024,7 @@
       <c r="AA15" s="6"/>
       <c r="AB15" s="6"/>
     </row>
-    <row r="16" spans="1:28" ht="16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>306</v>
       </c>
@@ -9064,21 +9064,21 @@
       <c r="AA16" s="6"/>
       <c r="AB16" s="6"/>
     </row>
-    <row r="17" spans="1:12" ht="16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>341</v>
+      </c>
+      <c r="B17" t="s">
+        <v>341</v>
+      </c>
+      <c r="C17" t="s">
         <v>342</v>
-      </c>
-      <c r="B17" t="s">
-        <v>342</v>
-      </c>
-      <c r="C17" t="s">
-        <v>343</v>
       </c>
       <c r="D17" s="16" t="s">
         <v>216</v>
       </c>
       <c r="L17" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
   </sheetData>
@@ -9100,12 +9100,12 @@
   <dimension ref="A1:AB10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -9114,7 +9114,7 @@
       </c>
       <c r="C1" s="5"/>
     </row>
-    <row r="2" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -9123,16 +9123,16 @@
       </c>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>332</v>
+        <v>343</v>
       </c>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -9141,25 +9141,25 @@
       </c>
       <c r="C4" s="14"/>
     </row>
-    <row r="5" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C5" s="14"/>
     </row>
-    <row r="6" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C6" s="14"/>
     </row>
-    <row r="7" spans="1:28" ht="16.5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:28" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -9383,16 +9383,16 @@
   <sheetPr codeName="Hoja16"/>
   <dimension ref="A1:AB33"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.36328125" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.33203125" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>5</v>
       </c>
@@ -9402,7 +9402,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
@@ -9412,17 +9412,17 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>332</v>
+        <v>343</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -9432,27 +9432,27 @@
       <c r="C4" s="17"/>
       <c r="D4" s="17"/>
     </row>
-    <row r="5" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C5" s="17"/>
       <c r="D5" s="17"/>
     </row>
-    <row r="6" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>
     </row>
-    <row r="7" spans="1:28" ht="16.5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:28" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
         <v>8</v>
       </c>
@@ -10595,17 +10595,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AB13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.90625" customWidth="1"/>
-    <col min="2" max="2" width="22.453125" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" customWidth="1"/>
+    <col min="2" max="2" width="22.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -10614,7 +10614,7 @@
       </c>
       <c r="C1" s="5"/>
     </row>
-    <row r="2" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -10623,16 +10623,16 @@
       </c>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>332</v>
+        <v>343</v>
       </c>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -10641,25 +10641,25 @@
       </c>
       <c r="C4" s="14"/>
     </row>
-    <row r="5" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C5" s="14"/>
     </row>
-    <row r="6" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C6" s="14"/>
     </row>
-    <row r="7" spans="1:28" ht="16.5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:28" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -11008,12 +11008,12 @@
       <selection activeCell="A8" sqref="A8:A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -11022,7 +11022,7 @@
       </c>
       <c r="C1" s="5"/>
     </row>
-    <row r="2" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -11031,7 +11031,7 @@
       </c>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -11040,7 +11040,7 @@
       </c>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -11049,7 +11049,7 @@
       </c>
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -11058,7 +11058,7 @@
       </c>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -11067,7 +11067,7 @@
       </c>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -11076,7 +11076,7 @@
       </c>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -11085,7 +11085,7 @@
       </c>
       <c r="C8" s="5"/>
     </row>
-    <row r="9" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -11115,13 +11115,13 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.453125" customWidth="1"/>
-    <col min="2" max="2" width="40.08984375" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" customWidth="1"/>
+    <col min="2" max="2" width="40.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -11131,7 +11131,7 @@
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
     </row>
-    <row r="2" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -11141,7 +11141,7 @@
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
     </row>
-    <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -11151,7 +11151,7 @@
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -11161,7 +11161,7 @@
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -11171,7 +11171,7 @@
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
     </row>
-    <row r="6" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -11181,7 +11181,7 @@
       <c r="C6" s="14"/>
       <c r="D6" s="21"/>
     </row>
-    <row r="7" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -11191,7 +11191,7 @@
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
     </row>
-    <row r="8" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -11201,7 +11201,7 @@
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
     </row>
-    <row r="9" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -11230,17 +11230,17 @@
   <dimension ref="A1:AB18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.08984375" customWidth="1"/>
-    <col min="2" max="2" width="30.54296875" customWidth="1"/>
-    <col min="4" max="4" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.109375" customWidth="1"/>
+    <col min="2" max="2" width="30.5546875" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -11250,7 +11250,7 @@
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
     </row>
-    <row r="2" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -11260,17 +11260,17 @@
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
     </row>
-    <row r="3" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>332</v>
+        <v>343</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -11280,27 +11280,27 @@
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
     </row>
-    <row r="5" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
     </row>
-    <row r="6" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
     </row>
-    <row r="7" spans="1:28" ht="16.5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:28" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -11802,12 +11802,12 @@
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.54296875" customWidth="1"/>
+    <col min="1" max="1" width="21.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -11817,7 +11817,7 @@
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
     </row>
-    <row r="2" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -11827,7 +11827,7 @@
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
     </row>
-    <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -11837,7 +11837,7 @@
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -11847,7 +11847,7 @@
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -11857,7 +11857,7 @@
       <c r="C5" s="15"/>
       <c r="D5" s="15"/>
     </row>
-    <row r="6" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -11867,7 +11867,7 @@
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
     </row>
-    <row r="7" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -11877,7 +11877,7 @@
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
     </row>
-    <row r="8" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -11887,7 +11887,7 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -11918,15 +11918,15 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.90625" customWidth="1"/>
-    <col min="2" max="2" width="26.08984375" customWidth="1"/>
-    <col min="3" max="3" width="24.54296875" customWidth="1"/>
-    <col min="4" max="4" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" customWidth="1"/>
+    <col min="2" max="2" width="26.109375" customWidth="1"/>
+    <col min="3" max="3" width="24.5546875" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -11936,7 +11936,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -11946,7 +11946,7 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -11956,7 +11956,7 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -11966,7 +11966,7 @@
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -11976,7 +11976,7 @@
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
     </row>
-    <row r="6" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -11986,7 +11986,7 @@
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
     </row>
-    <row r="7" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -11996,7 +11996,7 @@
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
     </row>
-    <row r="8" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -12004,7 +12004,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -12033,14 +12033,14 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="2" width="21.08984375" customWidth="1"/>
-    <col min="4" max="4" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.109375" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -12050,7 +12050,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -12060,7 +12060,7 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -12070,7 +12070,7 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -12080,7 +12080,7 @@
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -12090,7 +12090,7 @@
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
     </row>
-    <row r="6" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -12100,7 +12100,7 @@
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
     </row>
-    <row r="7" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -12110,7 +12110,7 @@
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
     </row>
-    <row r="8" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -12120,7 +12120,7 @@
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
     </row>
-    <row r="9" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -12148,15 +12148,15 @@
   <dimension ref="A1:AB12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -12166,7 +12166,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -12176,17 +12176,17 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>332</v>
+        <v>343</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -12196,27 +12196,27 @@
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
     </row>
-    <row r="5" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
     </row>
-    <row r="6" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
     </row>
-    <row r="7" spans="1:28" ht="16.5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:28" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -12516,12 +12516,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -12697,15 +12694,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{742639C9-D5E0-4CBF-8139-6F41798C6819}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E61FB905-6753-4D6B-9555-45A818BB6BAA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="541a8a8b-b856-4d35-a5c7-7f2c0ec3d499"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -12729,17 +12737,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E61FB905-6753-4D6B-9555-45A818BB6BAA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{742639C9-D5E0-4CBF-8139-6F41798C6819}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="541a8a8b-b856-4d35-a5c7-7f2c0ec3d499"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated version in technical codelists for 3.2.0 release (update)
</commit_message>
<xml_diff>
--- a/__ESPDTeam__/ESPD-CodeLists.xlsx
+++ b/__ESPDTeam__/ESPD-CodeLists.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\JC\Proyectos\17 - OP - ESPD\ESPD-EDM\__ESPDTeam__\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\JC\Proyectos\17 - OP - ESPD\TEDSPD-498\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD7B995D-B373-46EA-B8BD-EC29B48D6AF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36E0789E-A70E-4D7E-B6F7-B37AA91358FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="884" firstSheet="7" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="884" firstSheet="7" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AccessRight" sheetId="199" r:id="rId1"/>
@@ -308,7 +308,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="941" uniqueCount="346">
   <si>
     <t>ListID</t>
   </si>
@@ -1324,9 +1324,6 @@
     <t>https://github.com/ESPD/ESPD-EDM/tree/v3.1.0/codelists/gc/FinancialRatioType.gc</t>
   </si>
   <si>
-    <t>https://github.com/ESPD/ESPD-EDM/tree/v3.1.0/codelists/gc/ProfileExecutionID.gc</t>
-  </si>
-  <si>
     <t>https://github.com/ESPD/ESPD-EDM/tree/v3.1.0/codelists/gc/PropertyGroupType.gc</t>
   </si>
   <si>
@@ -1340,6 +1337,15 @@
   </si>
   <si>
     <t>3.2.0</t>
+  </si>
+  <si>
+    <t>https://github.com/ESPD/ESPD-EDM/tree/v3.2.0</t>
+  </si>
+  <si>
+    <t>https://github.com/ESPD/ESPD-EDM/tree/v3.2.0/codelists/gc/ProfileExecutionID.gc</t>
+  </si>
+  <si>
+    <t>ESPD-EDMv3.2.0</t>
   </si>
 </sst>
 </file>
@@ -6542,8 +6548,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF19000000}" name="Table7837136211455221705220992219922300224013" displayName="Table7837136211455221705220992219922300224013" ref="A7:AB17" tableType="xml" totalsRowShown="0" connectionId="66">
-  <autoFilter ref="A7:AB17" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF19000000}" name="Table7837136211455221705220992219922300224013" displayName="Table7837136211455221705220992219922300224013" ref="A7:AB18" tableType="xml" totalsRowShown="0" connectionId="66">
+  <autoFilter ref="A7:AB18" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A12:B41">
     <sortCondition ref="A12"/>
   </sortState>
@@ -7471,7 +7477,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
@@ -8703,10 +8709,10 @@
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <sheetPr codeName="Hoja13"/>
-  <dimension ref="A1:AB17"/>
+  <dimension ref="A1:AB18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -8740,7 +8746,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -8760,7 +8766,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>332</v>
+        <v>343</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -8770,7 +8776,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>338</v>
+        <v>344</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -9066,19 +9072,36 @@
     </row>
     <row r="17" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>340</v>
+      </c>
+      <c r="B17" t="s">
+        <v>340</v>
+      </c>
+      <c r="C17" t="s">
         <v>341</v>
-      </c>
-      <c r="B17" t="s">
-        <v>341</v>
-      </c>
-      <c r="C17" t="s">
-        <v>342</v>
       </c>
       <c r="D17" s="16" t="s">
         <v>216</v>
       </c>
       <c r="L17" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>345</v>
+      </c>
+      <c r="B18" t="s">
+        <v>345</v>
+      </c>
+      <c r="C18" t="s">
         <v>341</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>216</v>
+      </c>
+      <c r="L18" t="s">
+        <v>345</v>
       </c>
     </row>
   </sheetData>
@@ -9128,7 +9151,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C3" s="5"/>
     </row>
@@ -9155,7 +9178,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C6" s="14"/>
     </row>
@@ -9383,7 +9406,7 @@
   <sheetPr codeName="Hoja16"/>
   <dimension ref="A1:AB33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -9417,7 +9440,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -9447,7 +9470,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>
@@ -10628,7 +10651,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C3" s="5"/>
     </row>
@@ -11265,7 +11288,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -12181,7 +12204,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -12516,9 +12539,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -12694,26 +12720,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E61FB905-6753-4D6B-9555-45A818BB6BAA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{742639C9-D5E0-4CBF-8139-6F41798C6819}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="541a8a8b-b856-4d35-a5c7-7f2c0ec3d499"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -12737,9 +12752,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{742639C9-D5E0-4CBF-8139-6F41798C6819}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E61FB905-6753-4D6B-9555-45A818BB6BAA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="541a8a8b-b856-4d35-a5c7-7f2c0ec3d499"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated version in technical codelists for 3.2.0 release (new update)
</commit_message>
<xml_diff>
--- a/__ESPDTeam__/ESPD-CodeLists.xlsx
+++ b/__ESPDTeam__/ESPD-CodeLists.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\JC\Proyectos\17 - OP - ESPD\TEDSPD-498\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\JC\Proyectos\17 - OP - ESPD\ESPD-EDM\__ESPDTeam__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36E0789E-A70E-4D7E-B6F7-B37AA91358FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCB2396F-0B62-433D-A242-B45A0A75CD99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="884" firstSheet="7" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="884" firstSheet="7" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AccessRight" sheetId="199" r:id="rId1"/>
@@ -308,7 +308,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="941" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="941" uniqueCount="345">
   <si>
     <t>ListID</t>
   </si>
@@ -1306,30 +1306,6 @@
     <t>http://publications.europa.eu/resource/authority/occupation</t>
   </si>
   <si>
-    <t>https://github.com/ESPD/ESPD-EDM/tree/v3.1.0</t>
-  </si>
-  <si>
-    <t>https://github.com/ESPD/ESPD-EDM/tree/v3.1.0/codelists/gc/CriterionElementType.gc</t>
-  </si>
-  <si>
-    <t>https://github.com/OP-TED/ESPD-EDM/tree/3.1.0/</t>
-  </si>
-  <si>
-    <t>https://github.com/ESPD/ESPD-EDM/tree/v3.1.0/codelists/gc/BooleanGUIControlType.gc</t>
-  </si>
-  <si>
-    <t>https://github.com/ESPD/ESPD-EDM/tree/v3.1.0/codelists/gc/EOIDType.gc</t>
-  </si>
-  <si>
-    <t>https://github.com/ESPD/ESPD-EDM/tree/v3.1.0/codelists/gc/FinancialRatioType.gc</t>
-  </si>
-  <si>
-    <t>https://github.com/ESPD/ESPD-EDM/tree/v3.1.0/codelists/gc/PropertyGroupType.gc</t>
-  </si>
-  <si>
-    <t>https://github.com/ESPD/ESPD-EDM/tree/v3.1.0/codelists/gc/ResponseDataType.gc</t>
-  </si>
-  <si>
     <t>ESPD-EDMv3.1.0</t>
   </si>
   <si>
@@ -1346,6 +1322,27 @@
   </si>
   <si>
     <t>ESPD-EDMv3.2.0</t>
+  </si>
+  <si>
+    <t>https://github.com/OP-TED/ESPD-EDM/tree/3.2.0/</t>
+  </si>
+  <si>
+    <t>https://github.com/ESPD/ESPD-EDM/tree/v3.2.0/codelists/gc/BooleanGUIControlType.gc</t>
+  </si>
+  <si>
+    <t>https://github.com/ESPD/ESPD-EDM/tree/v3.2.0/codelists/gc/CriterionElementType.gc</t>
+  </si>
+  <si>
+    <t>https://github.com/ESPD/ESPD-EDM/tree/v3.2.0/codelists/gc/EOIDType.gc</t>
+  </si>
+  <si>
+    <t>https://github.com/ESPD/ESPD-EDM/tree/v3.2.0/codelists/gc/FinancialRatioType.gc</t>
+  </si>
+  <si>
+    <t>https://github.com/ESPD/ESPD-EDM/tree/v3.2.0/codelists/gc/PropertyGroupType.gc</t>
+  </si>
+  <si>
+    <t>https://github.com/ESPD/ESPD-EDM/tree/v3.2.0/codelists/gc/ResponseDataType.gc</t>
   </si>
 </sst>
 </file>
@@ -7477,7 +7474,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
@@ -7493,7 +7490,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
@@ -7501,7 +7498,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>337</v>
+        <v>342</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
@@ -8711,7 +8708,7 @@
   <sheetPr codeName="Hoja13"/>
   <dimension ref="A1:AB18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
@@ -8746,7 +8743,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -8766,7 +8763,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -8776,7 +8773,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -9072,36 +9069,36 @@
     </row>
     <row r="17" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="B17" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="C17" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="D17" s="16" t="s">
         <v>216</v>
       </c>
       <c r="L17" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="B18" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="C18" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="D18" s="16" t="s">
         <v>216</v>
       </c>
       <c r="L18" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
     </row>
   </sheetData>
@@ -9151,7 +9148,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="C3" s="5"/>
     </row>
@@ -9169,7 +9166,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="C5" s="14"/>
     </row>
@@ -9178,7 +9175,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>338</v>
+        <v>343</v>
       </c>
       <c r="C6" s="14"/>
     </row>
@@ -9406,7 +9403,7 @@
   <sheetPr codeName="Hoja16"/>
   <dimension ref="A1:AB33"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -9440,7 +9437,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -9460,7 +9457,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="C5" s="17"/>
       <c r="D5" s="17"/>
@@ -9470,7 +9467,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>339</v>
+        <v>344</v>
       </c>
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>
@@ -10619,7 +10616,7 @@
   <dimension ref="A1:AB13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -10651,7 +10648,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="C3" s="5"/>
     </row>
@@ -10669,7 +10666,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="C5" s="14"/>
     </row>
@@ -10678,7 +10675,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="C6" s="14"/>
     </row>
@@ -11253,7 +11250,7 @@
   <dimension ref="A1:AB18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -11288,7 +11285,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -11308,7 +11305,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -11318,7 +11315,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>333</v>
+        <v>340</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -12204,7 +12201,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -12224,7 +12221,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -12234,7 +12231,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>336</v>
+        <v>341</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -12539,12 +12536,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -12720,15 +12714,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{742639C9-D5E0-4CBF-8139-6F41798C6819}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E61FB905-6753-4D6B-9555-45A818BB6BAA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="541a8a8b-b856-4d35-a5c7-7f2c0ec3d499"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -12752,17 +12757,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E61FB905-6753-4D6B-9555-45A818BB6BAA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{742639C9-D5E0-4CBF-8139-6F41798C6819}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="541a8a8b-b856-4d35-a5c7-7f2c0ec3d499"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fix TEDSPD-548 #348 and Fix TEDSPD-222 #325
Fix TEDSPD-548 #348 and Fix TEDSPD-222 #325

Latest codelists for Occupation and Criterion downloaded from EU Vocabularies.

Corresponding version updated in ESPD-Codelists and XSLT files.
</commit_message>
<xml_diff>
--- a/__ESPDTeam__/ESPD-CodeLists.xlsx
+++ b/__ESPDTeam__/ESPD-CodeLists.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\JC\Proyectos\17 - OP - ESPD\ESPD-EDM\__ESPDTeam__\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ptchiene\OneDrive - NTT DATA EMEAL\Documents\GitHub\ESPD-EDM\__ESPDTeam__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCB2396F-0B62-433D-A242-B45A0A75CD99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{680C8D38-0EF2-4693-B574-C1F57054597F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="884" firstSheet="7" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="884" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AccessRight" sheetId="199" r:id="rId1"/>
@@ -1186,15 +1186,6 @@
     <t>financial-ratio-type</t>
   </si>
   <si>
-    <t>20210616-0</t>
-  </si>
-  <si>
-    <t>http://publications.europa.eu/resource/dataset/criterion/20210616-0</t>
-  </si>
-  <si>
-    <t>http://publications.europa.eu/resource/distribution/criterion/20210616-0/xml/gc/Criterion.gc</t>
-  </si>
-  <si>
     <t>20211208-0</t>
   </si>
   <si>
@@ -1237,18 +1228,9 @@
     <t>Date values (format YYYY-MM-DD)</t>
   </si>
   <si>
-    <t>20220615-0</t>
-  </si>
-  <si>
     <t>http://publications.europa.eu/resource/dataset/occupation</t>
   </si>
   <si>
-    <t>http://publications.europa.eu/resource/dataset/occupation/20220615-0</t>
-  </si>
-  <si>
-    <t>http://publications.europa.eu/resource/distribution/occupation/20220615-0/xml/gc/Occupation.gc</t>
-  </si>
-  <si>
     <t>20220928-0</t>
   </si>
   <si>
@@ -1343,13 +1325,31 @@
   </si>
   <si>
     <t>https://github.com/ESPD/ESPD-EDM/tree/v3.2.0/codelists/gc/ResponseDataType.gc</t>
+  </si>
+  <si>
+    <t>20230315-0</t>
+  </si>
+  <si>
+    <t>http://publications.europa.eu/resource/dataset/criterion/20230315-0</t>
+  </si>
+  <si>
+    <t>http://publications.europa.eu/resource/distribution/criterion/20230315-0/xml/gc/Criterion.gc</t>
+  </si>
+  <si>
+    <t>20221214-0</t>
+  </si>
+  <si>
+    <t>http://publications.europa.eu/resource/dataset/occupation/20221214-0</t>
+  </si>
+  <si>
+    <t>http://publications.europa.eu/resource/distribution/occupation/20221214-0/xml/gc/Occupation.gc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1572,7 +1572,7 @@
     <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Hipervínculo" xfId="4" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
     <cellStyle name="Nor_x0004_al" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
@@ -6770,7 +6770,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -7097,9 +7097,9 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="15.6328125" defaultRowHeight="12.5"/>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" ht="13">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -7108,7 +7108,7 @@
       </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="13">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -7117,7 +7117,7 @@
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" ht="13">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -7126,16 +7126,16 @@
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" ht="13">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" ht="13">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -7144,26 +7144,26 @@
       </c>
       <c r="C5" s="14"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" ht="13">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="C6" s="14"/>
       <c r="F6" s="21"/>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" ht="13">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="C7" s="14"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" ht="13">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -7172,7 +7172,7 @@
       </c>
       <c r="C8" s="5"/>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" ht="13">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -7181,7 +7181,7 @@
       </c>
       <c r="C9" s="5"/>
     </row>
-    <row r="10" spans="1:28" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:28" ht="14">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -7267,60 +7267,60 @@
         <v>201</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28">
       <c r="A11" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="D11" t="s">
         <v>216</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="L11" s="6" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28">
+      <c r="A12" t="s">
+        <v>298</v>
+      </c>
+      <c r="B12" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>301</v>
-      </c>
-      <c r="B12" t="s">
-        <v>302</v>
-      </c>
       <c r="C12" s="6" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D12" t="s">
         <v>216</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="L12" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28">
       <c r="C13" s="6"/>
       <c r="J13" s="6"/>
     </row>
-    <row r="14" spans="1:28" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" ht="16">
       <c r="D14" s="16"/>
     </row>
-    <row r="15" spans="1:28" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" ht="16">
       <c r="D15" s="16"/>
     </row>
-    <row r="16" spans="1:28" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" ht="16">
       <c r="D16" s="16"/>
     </row>
-    <row r="17" spans="4:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:4" ht="16">
       <c r="D17" s="16"/>
     </row>
   </sheetData>
@@ -7347,15 +7347,15 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="15.6328125" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" customWidth="1"/>
+    <col min="1" max="1" width="23.36328125" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="33.5546875" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.54296875" customWidth="1"/>
+    <col min="4" max="4" width="8.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="13">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -7363,7 +7363,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="13">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -7371,7 +7371,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="13">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -7379,15 +7379,15 @@
         <v>272</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="13">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="13">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -7395,23 +7395,23 @@
         <v>271</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="13">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="13">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="13">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -7419,7 +7419,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="13">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -7448,12 +7448,12 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="15.6328125" defaultRowHeight="12.5"/>
   <cols>
-    <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" ht="13">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -7461,7 +7461,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="13">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -7469,15 +7469,15 @@
         <v>291</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" ht="13">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" ht="13">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -7485,23 +7485,23 @@
         <v>203</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" ht="13">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" ht="13">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" ht="13">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
@@ -7509,7 +7509,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" ht="13">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
@@ -7517,7 +7517,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:28" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:28" ht="14">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -7603,7 +7603,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28">
       <c r="A10" s="3" t="s">
         <v>50</v>
       </c>
@@ -7621,7 +7621,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28">
       <c r="A11" s="3" t="s">
         <v>51</v>
       </c>
@@ -7638,7 +7638,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28">
       <c r="A12" s="3" t="s">
         <v>52</v>
       </c>
@@ -7655,7 +7655,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28">
       <c r="A13" s="3" t="s">
         <v>53</v>
       </c>
@@ -7672,7 +7672,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28">
       <c r="A14" s="3" t="s">
         <v>54</v>
       </c>
@@ -7689,7 +7689,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28">
       <c r="A15" s="3" t="s">
         <v>55</v>
       </c>
@@ -7706,7 +7706,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28">
       <c r="A16" s="3" t="s">
         <v>68</v>
       </c>
@@ -7723,7 +7723,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28">
       <c r="A17" s="3" t="s">
         <v>69</v>
       </c>
@@ -7740,7 +7740,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28">
       <c r="A18" s="3" t="s">
         <v>70</v>
       </c>
@@ -7757,7 +7757,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28">
       <c r="A19" s="3" t="s">
         <v>71</v>
       </c>
@@ -7774,7 +7774,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28">
       <c r="A20" s="3" t="s">
         <v>72</v>
       </c>
@@ -7791,7 +7791,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28">
       <c r="A21" s="3" t="s">
         <v>73</v>
       </c>
@@ -7808,7 +7808,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28">
       <c r="A22" s="3" t="s">
         <v>74</v>
       </c>
@@ -7825,7 +7825,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28">
       <c r="A23" s="3" t="s">
         <v>87</v>
       </c>
@@ -7849,7 +7849,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:28">
       <c r="A24" s="3" t="s">
         <v>88</v>
       </c>
@@ -7889,7 +7889,7 @@
       <c r="AA24" s="6"/>
       <c r="AB24" s="6"/>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:28">
       <c r="A25" s="3" t="s">
         <v>89</v>
       </c>
@@ -7929,7 +7929,7 @@
       <c r="AA25" s="6"/>
       <c r="AB25" s="6"/>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:28">
       <c r="A26" s="3" t="s">
         <v>90</v>
       </c>
@@ -7969,7 +7969,7 @@
       <c r="AA26" s="6"/>
       <c r="AB26" s="6"/>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:28">
       <c r="A27" s="3" t="s">
         <v>91</v>
       </c>
@@ -8009,7 +8009,7 @@
       <c r="AA27" s="6"/>
       <c r="AB27" s="6"/>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28">
       <c r="A28" s="3" t="s">
         <v>92</v>
       </c>
@@ -8049,7 +8049,7 @@
       <c r="AA28" s="6"/>
       <c r="AB28" s="6"/>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28">
       <c r="A29" s="3" t="s">
         <v>93</v>
       </c>
@@ -8089,7 +8089,7 @@
       <c r="AA29" s="6"/>
       <c r="AB29" s="6"/>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28">
       <c r="A30" s="3" t="s">
         <v>94</v>
       </c>
@@ -8129,7 +8129,7 @@
       <c r="AA30" s="6"/>
       <c r="AB30" s="6"/>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:28">
       <c r="A31" s="3" t="s">
         <v>95</v>
       </c>
@@ -8169,7 +8169,7 @@
       <c r="AA31" s="6"/>
       <c r="AB31" s="6"/>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:28">
       <c r="A32" s="3" t="s">
         <v>96</v>
       </c>
@@ -8209,7 +8209,7 @@
       <c r="AA32" s="6"/>
       <c r="AB32" s="6"/>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:28">
       <c r="A33" s="7" t="s">
         <v>112</v>
       </c>
@@ -8249,7 +8249,7 @@
       <c r="AA33" s="6"/>
       <c r="AB33" s="6"/>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:28">
       <c r="A34" s="7" t="s">
         <v>113</v>
       </c>
@@ -8289,7 +8289,7 @@
       <c r="AA34" s="6"/>
       <c r="AB34" s="6"/>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:28">
       <c r="A35" s="7" t="s">
         <v>118</v>
       </c>
@@ -8329,7 +8329,7 @@
       <c r="AA35" s="6"/>
       <c r="AB35" s="6"/>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:28">
       <c r="A36" s="7" t="s">
         <v>119</v>
       </c>
@@ -8369,7 +8369,7 @@
       <c r="AA36" s="6"/>
       <c r="AB36" s="6"/>
     </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:28">
       <c r="A37" s="7" t="s">
         <v>120</v>
       </c>
@@ -8409,7 +8409,7 @@
       <c r="AA37" s="6"/>
       <c r="AB37" s="6"/>
     </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:28">
       <c r="A38" s="7" t="s">
         <v>121</v>
       </c>
@@ -8473,13 +8473,13 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="15.6328125" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.90625" customWidth="1"/>
+    <col min="4" max="4" width="8.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="13">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -8488,7 +8488,7 @@
       </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="13">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -8497,7 +8497,7 @@
       </c>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="13">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -8505,16 +8505,16 @@
         <v>279</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="13">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="13">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -8523,25 +8523,25 @@
       </c>
       <c r="C5" s="14"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="13">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="C6" s="14"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="13">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="C7" s="14"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="13">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -8550,7 +8550,7 @@
       </c>
       <c r="C8" s="5"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="13">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -8576,17 +8576,17 @@
   <dimension ref="A1:AB9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="15.6328125" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" customWidth="1"/>
-    <col min="2" max="2" width="22.44140625" customWidth="1"/>
-    <col min="3" max="3" width="18.5546875" customWidth="1"/>
+    <col min="1" max="1" width="19.90625" customWidth="1"/>
+    <col min="2" max="2" width="22.453125" customWidth="1"/>
+    <col min="3" max="3" width="18.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" ht="13">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -8595,7 +8595,7 @@
       </c>
       <c r="C1" s="5"/>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="13">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -8604,57 +8604,57 @@
       </c>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" ht="13">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" ht="13">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>309</v>
+        <v>342</v>
       </c>
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" ht="13">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="C5" s="14"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" ht="13">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>311</v>
+        <v>343</v>
       </c>
       <c r="C6" s="14"/>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" ht="13">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>312</v>
+        <v>344</v>
       </c>
       <c r="C7" s="14"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" ht="13">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
@@ -8683,12 +8683,12 @@
       <c r="AA8" s="6"/>
       <c r="AB8" s="6"/>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" ht="13">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
     </row>
   </sheetData>
@@ -8712,13 +8712,13 @@
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="27.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.44140625" customWidth="1"/>
+    <col min="1" max="1" width="27.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" ht="13">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -8728,7 +8728,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="13">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -8738,17 +8738,17 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" ht="13">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" ht="13">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -8758,27 +8758,27 @@
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" ht="13">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" ht="13">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
     </row>
-    <row r="7" spans="1:28" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:28" ht="14">
       <c r="A7" s="8" t="s">
         <v>8</v>
       </c>
@@ -8864,7 +8864,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28">
       <c r="A8" t="s">
         <v>206</v>
       </c>
@@ -8882,7 +8882,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28">
       <c r="A9" t="s">
         <v>209</v>
       </c>
@@ -8899,7 +8899,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="10" spans="1:28" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" ht="16">
       <c r="A10" t="s">
         <v>242</v>
       </c>
@@ -8916,7 +8916,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="11" spans="1:28" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" ht="16">
       <c r="A11" t="s">
         <v>243</v>
       </c>
@@ -8934,7 +8934,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="12" spans="1:28" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" ht="16">
       <c r="A12" t="s">
         <v>212</v>
       </c>
@@ -8951,7 +8951,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="13" spans="1:28" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" ht="16">
       <c r="A13" t="s">
         <v>246</v>
       </c>
@@ -8970,7 +8970,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="14" spans="1:28" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" ht="16">
       <c r="A14" s="6" t="s">
         <v>249</v>
       </c>
@@ -8987,7 +8987,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="15" spans="1:28" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" ht="16">
       <c r="A15" s="6" t="s">
         <v>250</v>
       </c>
@@ -9027,15 +9027,15 @@
       <c r="AA15" s="6"/>
       <c r="AB15" s="6"/>
     </row>
-    <row r="16" spans="1:28" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" ht="16">
       <c r="A16" s="6" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D16" s="16" t="s">
         <v>216</v>
@@ -9048,7 +9048,7 @@
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
       <c r="L16" s="6" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="M16" s="6"/>
       <c r="N16" s="6"/>
@@ -9067,38 +9067,38 @@
       <c r="AA16" s="6"/>
       <c r="AB16" s="6"/>
     </row>
-    <row r="17" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="16">
       <c r="A17" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="B17" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="C17" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="D17" s="16" t="s">
         <v>216</v>
       </c>
       <c r="L17" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="16">
       <c r="A18" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="B18" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="C18" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="D18" s="16" t="s">
         <v>216</v>
       </c>
       <c r="L18" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
     </row>
   </sheetData>
@@ -9123,9 +9123,9 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="15.6328125" defaultRowHeight="12.5"/>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" ht="13">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -9134,7 +9134,7 @@
       </c>
       <c r="C1" s="5"/>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="13">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -9143,16 +9143,16 @@
       </c>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" ht="13">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" ht="13">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -9161,25 +9161,25 @@
       </c>
       <c r="C4" s="14"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" ht="13">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="C5" s="14"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" ht="13">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="C6" s="14"/>
     </row>
-    <row r="7" spans="1:28" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:28" ht="14">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -9265,7 +9265,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28">
       <c r="A8" s="12" t="s">
         <v>159</v>
       </c>
@@ -9305,7 +9305,7 @@
       <c r="AA8" s="6"/>
       <c r="AB8" s="6"/>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28">
       <c r="A9" s="12" t="s">
         <v>160</v>
       </c>
@@ -9345,7 +9345,7 @@
       <c r="AA9" s="6"/>
       <c r="AB9" s="6"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28">
       <c r="A10" s="12" t="s">
         <v>161</v>
       </c>
@@ -9403,16 +9403,16 @@
   <sheetPr codeName="Hoja16"/>
   <dimension ref="A1:AB33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="15.6328125" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="35.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.36328125" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" ht="13">
       <c r="A1" s="9" t="s">
         <v>5</v>
       </c>
@@ -9422,7 +9422,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="13">
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
@@ -9432,17 +9432,17 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" ht="13">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" ht="13">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -9452,27 +9452,27 @@
       <c r="C4" s="17"/>
       <c r="D4" s="17"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" ht="13">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="C5" s="17"/>
       <c r="D5" s="17"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" ht="13">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>
     </row>
-    <row r="7" spans="1:28" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:28" ht="14">
       <c r="A7" s="8" t="s">
         <v>8</v>
       </c>
@@ -9558,7 +9558,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28">
       <c r="A8" s="8" t="s">
         <v>11</v>
       </c>
@@ -9598,7 +9598,7 @@
       <c r="AA8" s="8"/>
       <c r="AB8" s="8"/>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28">
       <c r="A9" s="8" t="s">
         <v>16</v>
       </c>
@@ -9638,7 +9638,7 @@
       <c r="AA9" s="8"/>
       <c r="AB9" s="8"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28">
       <c r="A10" s="8" t="s">
         <v>18</v>
       </c>
@@ -9678,15 +9678,15 @@
       <c r="AA10" s="8"/>
       <c r="AB10" s="8"/>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28">
       <c r="A11" s="8" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>216</v>
@@ -9699,7 +9699,7 @@
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
       <c r="L11" s="8" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="M11" s="8"/>
       <c r="N11" s="8"/>
@@ -9718,7 +9718,7 @@
       <c r="AA11" s="8"/>
       <c r="AB11" s="8"/>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28">
       <c r="A12" s="8" t="s">
         <v>10</v>
       </c>
@@ -9758,7 +9758,7 @@
       <c r="AA12" s="8"/>
       <c r="AB12" s="8"/>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28">
       <c r="A13" s="10" t="s">
         <v>166</v>
       </c>
@@ -9798,7 +9798,7 @@
       <c r="AA13" s="8"/>
       <c r="AB13" s="8"/>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28">
       <c r="A14" s="8" t="s">
         <v>21</v>
       </c>
@@ -9838,7 +9838,7 @@
       <c r="AA14" s="8"/>
       <c r="AB14" s="8"/>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28">
       <c r="A15" s="8" t="s">
         <v>23</v>
       </c>
@@ -9878,7 +9878,7 @@
       <c r="AA15" s="8"/>
       <c r="AB15" s="8"/>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28">
       <c r="A16" s="8" t="s">
         <v>13</v>
       </c>
@@ -9918,7 +9918,7 @@
       <c r="AA16" s="8"/>
       <c r="AB16" s="8"/>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28">
       <c r="A17" s="10" t="s">
         <v>26</v>
       </c>
@@ -9958,7 +9958,7 @@
       <c r="AA17" s="8"/>
       <c r="AB17" s="8"/>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28">
       <c r="A18" s="8" t="s">
         <v>28</v>
       </c>
@@ -9998,7 +9998,7 @@
       <c r="AA18" s="8"/>
       <c r="AB18" s="8"/>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28">
       <c r="A19" s="8" t="s">
         <v>30</v>
       </c>
@@ -10038,7 +10038,7 @@
       <c r="AA19" s="8"/>
       <c r="AB19" s="8"/>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28">
       <c r="A20" s="8" t="s">
         <v>34</v>
       </c>
@@ -10078,7 +10078,7 @@
       <c r="AA20" s="8"/>
       <c r="AB20" s="8"/>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28">
       <c r="A21" s="8" t="s">
         <v>47</v>
       </c>
@@ -10118,7 +10118,7 @@
       <c r="AA21" s="8"/>
       <c r="AB21" s="8"/>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28">
       <c r="A22" s="8" t="s">
         <v>128</v>
       </c>
@@ -10158,7 +10158,7 @@
       <c r="AA22" s="8"/>
       <c r="AB22" s="8"/>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28">
       <c r="A23" s="10" t="s">
         <v>134</v>
       </c>
@@ -10198,7 +10198,7 @@
       <c r="AA23" s="18"/>
       <c r="AB23" s="18"/>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:28">
       <c r="A24" s="10" t="s">
         <v>135</v>
       </c>
@@ -10238,7 +10238,7 @@
       <c r="AA24" s="18"/>
       <c r="AB24" s="18"/>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:28">
       <c r="A25" s="10" t="s">
         <v>136</v>
       </c>
@@ -10278,7 +10278,7 @@
       <c r="AA25" s="10"/>
       <c r="AB25" s="10"/>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:28">
       <c r="A26" s="10" t="s">
         <v>137</v>
       </c>
@@ -10318,7 +10318,7 @@
       <c r="AA26" s="10"/>
       <c r="AB26" s="10"/>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:28">
       <c r="A27" s="10" t="s">
         <v>138</v>
       </c>
@@ -10358,7 +10358,7 @@
       <c r="AA27" s="10"/>
       <c r="AB27" s="10"/>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28">
       <c r="A28" s="10" t="s">
         <v>139</v>
       </c>
@@ -10398,7 +10398,7 @@
       <c r="AA28" s="10"/>
       <c r="AB28" s="10"/>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28">
       <c r="A29" s="10" t="s">
         <v>140</v>
       </c>
@@ -10438,7 +10438,7 @@
       <c r="AA29" s="10"/>
       <c r="AB29" s="10"/>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28">
       <c r="A30" s="10" t="s">
         <v>148</v>
       </c>
@@ -10478,7 +10478,7 @@
       <c r="AA30" s="10"/>
       <c r="AB30" s="10"/>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:28">
       <c r="A31" s="10" t="s">
         <v>217</v>
       </c>
@@ -10518,7 +10518,7 @@
       <c r="AA31" s="10"/>
       <c r="AB31" s="10"/>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:28">
       <c r="A32" s="10" t="s">
         <v>220</v>
       </c>
@@ -10558,7 +10558,7 @@
       <c r="AA32" s="10"/>
       <c r="AB32" s="10"/>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:28">
       <c r="A33" s="19" t="s">
         <v>240</v>
       </c>
@@ -10619,13 +10619,13 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="15.6328125" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" customWidth="1"/>
-    <col min="2" max="2" width="22.44140625" customWidth="1"/>
+    <col min="1" max="1" width="19.90625" customWidth="1"/>
+    <col min="2" max="2" width="22.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" ht="13">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -10634,7 +10634,7 @@
       </c>
       <c r="C1" s="5"/>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="13">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -10643,16 +10643,16 @@
       </c>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" ht="13">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" ht="13">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -10661,25 +10661,25 @@
       </c>
       <c r="C4" s="14"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" ht="13">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="C5" s="14"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" ht="13">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C6" s="14"/>
     </row>
-    <row r="7" spans="1:28" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:28" ht="14">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -10765,7 +10765,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28">
       <c r="A8" s="6" t="s">
         <v>222</v>
       </c>
@@ -10805,7 +10805,7 @@
       <c r="AA8" s="6"/>
       <c r="AB8" s="6"/>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28">
       <c r="A9" s="6" t="s">
         <v>225</v>
       </c>
@@ -10845,7 +10845,7 @@
       <c r="AA9" s="6"/>
       <c r="AB9" s="6"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28">
       <c r="A10" s="6" t="s">
         <v>228</v>
       </c>
@@ -10885,7 +10885,7 @@
       <c r="AA10" s="6"/>
       <c r="AB10" s="6"/>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28">
       <c r="A11" t="s">
         <v>231</v>
       </c>
@@ -10925,7 +10925,7 @@
       <c r="AA11" s="6"/>
       <c r="AB11" s="6"/>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28">
       <c r="A12" s="6" t="s">
         <v>234</v>
       </c>
@@ -10965,7 +10965,7 @@
       <c r="AA12" s="6"/>
       <c r="AB12" s="6"/>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28">
       <c r="A13" s="6" t="s">
         <v>237</v>
       </c>
@@ -11028,12 +11028,12 @@
       <selection activeCell="A8" sqref="A8:A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="15.6328125" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="13">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -11042,7 +11042,7 @@
       </c>
       <c r="C1" s="5"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="13">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -11051,7 +11051,7 @@
       </c>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="13">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -11060,16 +11060,16 @@
       </c>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="13">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="13">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -11078,25 +11078,25 @@
       </c>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="13">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="13">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="13">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -11105,7 +11105,7 @@
       </c>
       <c r="C8" s="5"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="13">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -11131,17 +11131,17 @@
   <sheetPr codeName="Hoja5"/>
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="15.6328125" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="19.44140625" customWidth="1"/>
-    <col min="2" max="2" width="40.109375" customWidth="1"/>
+    <col min="1" max="1" width="19.453125" customWidth="1"/>
+    <col min="2" max="2" width="40.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="13">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -11151,7 +11151,7 @@
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="13">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -11161,7 +11161,7 @@
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="13">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -11171,17 +11171,17 @@
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="13">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>292</v>
+        <v>339</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="13">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -11191,27 +11191,27 @@
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="13">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>293</v>
+        <v>340</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="21"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="13">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>294</v>
+        <v>341</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="13">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -11221,7 +11221,7 @@
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="13">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -11231,7 +11231,7 @@
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
     </row>
-    <row r="10" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:4" s="20" customFormat="1" ht="13.25"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
@@ -11253,14 +11253,14 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="15.6328125" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="22.109375" customWidth="1"/>
-    <col min="2" max="2" width="30.5546875" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.08984375" customWidth="1"/>
+    <col min="2" max="2" width="30.54296875" customWidth="1"/>
+    <col min="4" max="4" width="8.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" ht="13">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -11270,7 +11270,7 @@
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="13">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -11280,17 +11280,17 @@
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" ht="13">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" ht="13">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -11300,27 +11300,27 @@
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" ht="13">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" ht="13">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
     </row>
-    <row r="7" spans="1:28" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:28" ht="14">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -11406,7 +11406,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28">
       <c r="A8" s="6" t="s">
         <v>126</v>
       </c>
@@ -11423,7 +11423,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28">
       <c r="A9" s="6" t="s">
         <v>151</v>
       </c>
@@ -11463,7 +11463,7 @@
       <c r="AA9" s="6"/>
       <c r="AB9" s="6"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28">
       <c r="A10" s="6" t="s">
         <v>130</v>
       </c>
@@ -11503,7 +11503,7 @@
       <c r="AA10" s="6"/>
       <c r="AB10" s="6"/>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28">
       <c r="A11" s="6" t="s">
         <v>150</v>
       </c>
@@ -11543,7 +11543,7 @@
       <c r="AA11" s="6"/>
       <c r="AB11" s="6"/>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28">
       <c r="A12" s="6" t="s">
         <v>131</v>
       </c>
@@ -11583,7 +11583,7 @@
       <c r="AA12" s="6"/>
       <c r="AB12" s="6"/>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28">
       <c r="A13" s="6" t="s">
         <v>132</v>
       </c>
@@ -11623,7 +11623,7 @@
       <c r="AA13" s="6"/>
       <c r="AB13" s="6"/>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28">
       <c r="A14" s="6" t="s">
         <v>152</v>
       </c>
@@ -11663,7 +11663,7 @@
       <c r="AA14" s="6"/>
       <c r="AB14" s="6"/>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28">
       <c r="A15" s="6" t="s">
         <v>133</v>
       </c>
@@ -11680,7 +11680,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28">
       <c r="A16" s="6" t="s">
         <v>153</v>
       </c>
@@ -11720,7 +11720,7 @@
       <c r="AA16" s="6"/>
       <c r="AB16" s="6"/>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28">
       <c r="A17" s="6" t="s">
         <v>155</v>
       </c>
@@ -11760,7 +11760,7 @@
       <c r="AA17" s="6"/>
       <c r="AB17" s="6"/>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28">
       <c r="A18" s="6" t="s">
         <v>156</v>
       </c>
@@ -11822,12 +11822,12 @@
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="15.6328125" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="21.5546875" customWidth="1"/>
+    <col min="1" max="1" width="21.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="13">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -11837,7 +11837,7 @@
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="13">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -11847,7 +11847,7 @@
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="13">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -11857,17 +11857,17 @@
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="13">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="13">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -11877,27 +11877,27 @@
       <c r="C5" s="15"/>
       <c r="D5" s="15"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="13">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="13">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="13">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -11907,7 +11907,7 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="13">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -11938,15 +11938,15 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="15.6328125" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" customWidth="1"/>
-    <col min="2" max="2" width="26.109375" customWidth="1"/>
-    <col min="3" max="3" width="24.5546875" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.90625" customWidth="1"/>
+    <col min="2" max="2" width="26.08984375" customWidth="1"/>
+    <col min="3" max="3" width="24.54296875" customWidth="1"/>
+    <col min="4" max="4" width="8.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="13">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -11956,7 +11956,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="13">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -11966,57 +11966,57 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="13">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="13">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="13">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="13">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="13">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="13">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -12024,7 +12024,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="13">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -12053,14 +12053,14 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="15.6328125" defaultRowHeight="12.5"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="2" width="21.109375" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.08984375" customWidth="1"/>
+    <col min="4" max="4" width="8.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="13">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -12070,7 +12070,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="13">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -12080,7 +12080,7 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="13">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -12090,17 +12090,17 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="13">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="13">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -12110,27 +12110,27 @@
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="13">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="13">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="13">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -12140,7 +12140,7 @@
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="13">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -12171,12 +12171,12 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="15.6328125" defaultRowHeight="12.5"/>
   <cols>
-    <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" ht="13">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -12186,7 +12186,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="13">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -12196,17 +12196,17 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" ht="13">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" ht="13">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -12216,27 +12216,27 @@
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" ht="13">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" ht="13">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
     </row>
-    <row r="7" spans="1:28" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:28" ht="14">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -12322,7 +12322,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -12362,7 +12362,7 @@
       <c r="AA8" s="4"/>
       <c r="AB8" s="4"/>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28">
       <c r="A9" t="s">
         <v>38</v>
       </c>
@@ -12402,7 +12402,7 @@
       <c r="AA9" s="4"/>
       <c r="AB9" s="4"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -12442,7 +12442,7 @@
       <c r="AA10" s="4"/>
       <c r="AB10" s="4"/>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -12482,7 +12482,7 @@
       <c r="AA11" s="4"/>
       <c r="AB11" s="4"/>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -12542,6 +12542,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100087E4EC354ADFB40AC5D4FC129E379BA" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="29f822455ff5391d2c7c2dfd7717ecba">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="541a8a8b-b856-4d35-a5c7-7f2c0ec3d499" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="35e6952e7efa586d011e824f69a654f2" ns2:_="">
     <xsd:import namespace="541a8a8b-b856-4d35-a5c7-7f2c0ec3d499"/>
@@ -12713,15 +12722,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E61FB905-6753-4D6B-9555-45A818BB6BAA}">
   <ds:schemaRefs>
@@ -12739,6 +12739,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{742639C9-D5E0-4CBF-8139-6F41798C6819}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5774DC4B-7AB9-4854-9E79-56DDD4D64737}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12754,12 +12762,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{742639C9-D5E0-4CBF-8139-6F41798C6819}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>